<commit_message>
[FEAT] add sort by research areas
</commit_message>
<xml_diff>
--- a/data/pubs.xlsx
+++ b/data/pubs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/DoerLBH/Dropbox (Personal)/Git/doerbeta.github.io/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{504FD7FD-03A0-2749-9B1E-9FE4135C1F3A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6742B94F-CB43-0742-B02D-E3FC302A38B4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="44080" yWindow="-5680" windowWidth="28040" windowHeight="17440" xr2:uid="{2388AA68-C25E-CF45-A9DC-089130C49FF2}"/>
+    <workbookView xWindow="47300" yWindow="-3340" windowWidth="28040" windowHeight="17440" xr2:uid="{2388AA68-C25E-CF45-A9DC-089130C49FF2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="255">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="282">
   <si>
     <t>title</t>
   </si>
@@ -545,9 +545,6 @@
     <t>Neural Networks as Model Selection with Incremental MDL Normalization</t>
   </si>
   <si>
-    <t>Nnmodelijcai</t>
-  </si>
-  <si>
     <t>IJCAI 2019 Workshop on Human Brain and Artificial Intelligence (HBAI)</t>
   </si>
   <si>
@@ -620,9 +617,6 @@
     <t>https://github.com/doerlbh/DREAM_PDBiomarker</t>
   </si>
   <si>
-    <t>Pdbiomarkerrsg</t>
-  </si>
-  <si>
     <t>RSG_PDBiomarker_poster.pdf</t>
   </si>
   <si>
@@ -798,6 +792,93 @@
   </si>
   <si>
     <t>Journal of Comparative Neurology</t>
+  </si>
+  <si>
+    <t>with</t>
+  </si>
+  <si>
+    <t>areas</t>
+  </si>
+  <si>
+    <t>self</t>
+  </si>
+  <si>
+    <t>SP-ML-HCI</t>
+  </si>
+  <si>
+    <t>kriegeskorte</t>
+  </si>
+  <si>
+    <t>ML-GT</t>
+  </si>
+  <si>
+    <t>ibm</t>
+  </si>
+  <si>
+    <t>ML-IT-CV</t>
+  </si>
+  <si>
+    <t>microsoft</t>
+  </si>
+  <si>
+    <t>NS-CV</t>
+  </si>
+  <si>
+    <t>ML-TM-NS</t>
+  </si>
+  <si>
+    <t>CV-HCI</t>
+  </si>
+  <si>
+    <t>self-kriegeskorte-rabadan</t>
+  </si>
+  <si>
+    <t>ML-GT-SB</t>
+  </si>
+  <si>
+    <t>olavarria</t>
+  </si>
+  <si>
+    <t>NS-ML</t>
+  </si>
+  <si>
+    <t>self-rabadan</t>
+  </si>
+  <si>
+    <t>baker</t>
+  </si>
+  <si>
+    <t>self-qian</t>
+  </si>
+  <si>
+    <t>SB</t>
+  </si>
+  <si>
+    <t>ML</t>
+  </si>
+  <si>
+    <t>peer</t>
+  </si>
+  <si>
+    <t>ML-SB-TM</t>
+  </si>
+  <si>
+    <t>NS-HCI</t>
+  </si>
+  <si>
+    <t>teng</t>
+  </si>
+  <si>
+    <t>ML-TM-AM</t>
+  </si>
+  <si>
+    <t>PDbiomarkerrsg</t>
+  </si>
+  <si>
+    <t>NNmodelijcai</t>
+  </si>
+  <si>
+    <t>ML-SB-TM-NS</t>
   </si>
 </sst>
 </file>
@@ -1160,10 +1241,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07DC3B69-47EC-374A-9EA9-8E92A8B21FEE}">
-  <dimension ref="A1:V26"/>
+  <dimension ref="A1:X26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="X25" sqref="X25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1173,7 +1254,7 @@
     <col min="8" max="8" width="28.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>30</v>
       </c>
@@ -1184,16 +1265,16 @@
         <v>26</v>
       </c>
       <c r="D1" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="E1" t="s">
         <v>11</v>
       </c>
       <c r="F1" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="G1" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="H1" t="s">
         <v>0</v>
@@ -1240,8 +1321,14 @@
       <c r="V1" t="s">
         <v>9</v>
       </c>
+      <c r="W1" t="s">
+        <v>253</v>
+      </c>
+      <c r="X1" t="s">
+        <v>254</v>
+      </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1282,8 +1369,14 @@
       <c r="V2" t="s">
         <v>21</v>
       </c>
+      <c r="W2" t="s">
+        <v>255</v>
+      </c>
+      <c r="X2" t="s">
+        <v>256</v>
+      </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1326,8 +1419,14 @@
       <c r="V3" t="s">
         <v>29</v>
       </c>
+      <c r="W3" t="s">
+        <v>255</v>
+      </c>
+      <c r="X3" t="s">
+        <v>256</v>
+      </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1</v>
       </c>
@@ -1365,8 +1464,14 @@
       <c r="V4" t="s">
         <v>38</v>
       </c>
+      <c r="W4" t="s">
+        <v>257</v>
+      </c>
+      <c r="X4" t="s">
+        <v>258</v>
+      </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1</v>
       </c>
@@ -1380,7 +1485,7 @@
         <v>13</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="G5">
         <v>1</v>
@@ -1410,8 +1515,14 @@
       <c r="V5" t="s">
         <v>46</v>
       </c>
+      <c r="W5" t="s">
+        <v>259</v>
+      </c>
+      <c r="X5" t="s">
+        <v>263</v>
+      </c>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>1</v>
       </c>
@@ -1451,8 +1562,14 @@
       <c r="V6" t="s">
         <v>49</v>
       </c>
+      <c r="W6" t="s">
+        <v>271</v>
+      </c>
+      <c r="X6" t="s">
+        <v>260</v>
+      </c>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>1</v>
       </c>
@@ -1480,8 +1597,14 @@
       <c r="V7" t="s">
         <v>60</v>
       </c>
+      <c r="W7" t="s">
+        <v>261</v>
+      </c>
+      <c r="X7" t="s">
+        <v>276</v>
+      </c>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>1</v>
       </c>
@@ -1498,7 +1621,7 @@
         <v>24</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="G8">
         <v>3</v>
@@ -1533,8 +1656,14 @@
       <c r="V8" t="s">
         <v>68</v>
       </c>
+      <c r="W8" t="s">
+        <v>259</v>
+      </c>
+      <c r="X8" t="s">
+        <v>263</v>
+      </c>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>1</v>
       </c>
@@ -1575,8 +1704,14 @@
       <c r="V9" t="s">
         <v>76</v>
       </c>
+      <c r="W9" t="s">
+        <v>255</v>
+      </c>
+      <c r="X9" t="s">
+        <v>264</v>
+      </c>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>1</v>
       </c>
@@ -1593,7 +1728,7 @@
         <v>24</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="G10">
         <v>3</v>
@@ -1628,8 +1763,14 @@
       <c r="V10" t="s">
         <v>94</v>
       </c>
+      <c r="W10" t="s">
+        <v>259</v>
+      </c>
+      <c r="X10" t="s">
+        <v>263</v>
+      </c>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>1</v>
       </c>
@@ -1672,8 +1813,14 @@
       <c r="V11" t="s">
         <v>102</v>
       </c>
+      <c r="W11" t="s">
+        <v>259</v>
+      </c>
+      <c r="X11" t="s">
+        <v>263</v>
+      </c>
     </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>1</v>
       </c>
@@ -1713,8 +1860,14 @@
       <c r="V12" t="s">
         <v>111</v>
       </c>
+      <c r="W12" t="s">
+        <v>265</v>
+      </c>
+      <c r="X12" t="s">
+        <v>266</v>
+      </c>
     </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>1</v>
       </c>
@@ -1737,7 +1890,7 @@
         <v>113</v>
       </c>
       <c r="J13" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="K13" t="s">
         <v>125</v>
@@ -1754,8 +1907,14 @@
       <c r="V13" t="s">
         <v>119</v>
       </c>
+      <c r="W13" t="s">
+        <v>267</v>
+      </c>
+      <c r="X13" t="s">
+        <v>262</v>
+      </c>
     </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>1</v>
       </c>
@@ -1795,8 +1954,14 @@
       <c r="V14" t="s">
         <v>123</v>
       </c>
+      <c r="W14" t="s">
+        <v>259</v>
+      </c>
+      <c r="X14" t="s">
+        <v>263</v>
+      </c>
     </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>1</v>
       </c>
@@ -1842,8 +2007,14 @@
       <c r="V15" t="s">
         <v>137</v>
       </c>
+      <c r="W15" t="s">
+        <v>257</v>
+      </c>
+      <c r="X15" t="s">
+        <v>268</v>
+      </c>
     </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>1</v>
       </c>
@@ -1889,8 +2060,14 @@
       <c r="V16" t="s">
         <v>111</v>
       </c>
+      <c r="W16" t="s">
+        <v>269</v>
+      </c>
+      <c r="X16" t="s">
+        <v>266</v>
+      </c>
     </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>1</v>
       </c>
@@ -1907,7 +2084,7 @@
         <v>114</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="G17">
         <v>6</v>
@@ -1942,8 +2119,14 @@
       <c r="V17" t="s">
         <v>158</v>
       </c>
+      <c r="W17" t="s">
+        <v>270</v>
+      </c>
+      <c r="X17" t="s">
+        <v>272</v>
+      </c>
     </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>1</v>
       </c>
@@ -1960,7 +2143,7 @@
         <v>24</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="G18">
         <v>3</v>
@@ -1995,13 +2178,19 @@
       <c r="V18" t="s">
         <v>163</v>
       </c>
+      <c r="W18" t="s">
+        <v>259</v>
+      </c>
+      <c r="X18" t="s">
+        <v>263</v>
+      </c>
     </row>
-    <row r="19" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>1</v>
       </c>
       <c r="B19" t="s">
-        <v>170</v>
+        <v>280</v>
       </c>
       <c r="C19">
         <v>2019</v>
@@ -2019,36 +2208,42 @@
         <v>48</v>
       </c>
       <c r="J19" t="s">
+        <v>170</v>
+      </c>
+      <c r="K19" t="s">
+        <v>176</v>
+      </c>
+      <c r="L19" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="K19" t="s">
-        <v>177</v>
-      </c>
-      <c r="L19" s="1" t="s">
+      <c r="M19" t="s">
+        <v>174</v>
+      </c>
+      <c r="P19" t="s">
+        <v>173</v>
+      </c>
+      <c r="R19" t="s">
         <v>172</v>
-      </c>
-      <c r="M19" t="s">
-        <v>175</v>
-      </c>
-      <c r="P19" t="s">
-        <v>174</v>
-      </c>
-      <c r="R19" t="s">
-        <v>173</v>
       </c>
       <c r="S19" s="1" t="s">
         <v>54</v>
       </c>
       <c r="V19" t="s">
-        <v>176</v>
+        <v>175</v>
+      </c>
+      <c r="W19" t="s">
+        <v>271</v>
+      </c>
+      <c r="X19" t="s">
+        <v>260</v>
       </c>
     </row>
-    <row r="20" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>1</v>
       </c>
       <c r="B20" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C20">
         <v>2018</v>
@@ -2060,42 +2255,48 @@
         <v>24</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="G20">
         <v>10</v>
       </c>
       <c r="H20" t="s">
+        <v>177</v>
+      </c>
+      <c r="I20" t="s">
         <v>178</v>
       </c>
-      <c r="I20" t="s">
+      <c r="J20" t="s">
         <v>179</v>
       </c>
-      <c r="J20" t="s">
+      <c r="K20" t="s">
+        <v>184</v>
+      </c>
+      <c r="L20" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="M20" t="s">
+        <v>182</v>
+      </c>
+      <c r="S20" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="V20" t="s">
         <v>180</v>
       </c>
-      <c r="K20" t="s">
-        <v>185</v>
-      </c>
-      <c r="L20" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="M20" t="s">
-        <v>183</v>
-      </c>
-      <c r="S20" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="V20" t="s">
-        <v>181</v>
+      <c r="W20" t="s">
+        <v>259</v>
+      </c>
+      <c r="X20" t="s">
+        <v>273</v>
       </c>
     </row>
-    <row r="21" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>1</v>
       </c>
       <c r="B21" t="s">
-        <v>195</v>
+        <v>279</v>
       </c>
       <c r="C21">
         <v>2017</v>
@@ -2107,42 +2308,48 @@
         <v>97</v>
       </c>
       <c r="H21" t="s">
+        <v>186</v>
+      </c>
+      <c r="I21" t="s">
         <v>187</v>
       </c>
-      <c r="I21" t="s">
+      <c r="J21" t="s">
+        <v>197</v>
+      </c>
+      <c r="K21" t="s">
+        <v>190</v>
+      </c>
+      <c r="L21" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="M21" t="s">
+        <v>189</v>
+      </c>
+      <c r="P21" t="s">
+        <v>194</v>
+      </c>
+      <c r="R21" t="s">
+        <v>192</v>
+      </c>
+      <c r="S21" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="V21" t="s">
         <v>188</v>
       </c>
-      <c r="J21" t="s">
-        <v>199</v>
-      </c>
-      <c r="K21" t="s">
-        <v>191</v>
-      </c>
-      <c r="L21" s="1" t="s">
-        <v>192</v>
-      </c>
-      <c r="M21" t="s">
-        <v>190</v>
-      </c>
-      <c r="P21" t="s">
-        <v>196</v>
-      </c>
-      <c r="R21" t="s">
-        <v>193</v>
-      </c>
-      <c r="S21" s="1" t="s">
-        <v>194</v>
-      </c>
-      <c r="V21" t="s">
-        <v>189</v>
+      <c r="W21" t="s">
+        <v>274</v>
+      </c>
+      <c r="X21" t="s">
+        <v>275</v>
       </c>
     </row>
-    <row r="22" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>1</v>
       </c>
       <c r="B22" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="C22">
         <v>2017</v>
@@ -2154,39 +2361,45 @@
         <v>114</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="G22">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="H22" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="I22" t="s">
+        <v>199</v>
+      </c>
+      <c r="J22" t="s">
+        <v>196</v>
+      </c>
+      <c r="K22" t="s">
+        <v>203</v>
+      </c>
+      <c r="M22" t="s">
         <v>201</v>
       </c>
-      <c r="J22" t="s">
+      <c r="Q22" t="s">
+        <v>200</v>
+      </c>
+      <c r="V22" t="s">
         <v>198</v>
       </c>
-      <c r="K22" t="s">
-        <v>205</v>
-      </c>
-      <c r="M22" t="s">
-        <v>203</v>
-      </c>
-      <c r="Q22" t="s">
-        <v>202</v>
-      </c>
-      <c r="V22" t="s">
-        <v>200</v>
+      <c r="W22" t="s">
+        <v>277</v>
+      </c>
+      <c r="X22" t="s">
+        <v>278</v>
       </c>
     </row>
-    <row r="23" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>1</v>
       </c>
       <c r="B23" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C23">
         <v>2017</v>
@@ -2198,39 +2411,45 @@
         <v>114</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="G23">
         <v>15</v>
       </c>
       <c r="H23" t="s">
+        <v>204</v>
+      </c>
+      <c r="I23" t="s">
         <v>206</v>
       </c>
-      <c r="I23" t="s">
-        <v>208</v>
-      </c>
       <c r="J23" t="s">
+        <v>205</v>
+      </c>
+      <c r="K23" t="s">
+        <v>209</v>
+      </c>
+      <c r="M23" t="s">
+        <v>211</v>
+      </c>
+      <c r="Q23" t="s">
+        <v>210</v>
+      </c>
+      <c r="V23" t="s">
         <v>207</v>
       </c>
-      <c r="K23" t="s">
-        <v>211</v>
-      </c>
-      <c r="M23" t="s">
-        <v>213</v>
-      </c>
-      <c r="Q23" t="s">
-        <v>212</v>
-      </c>
-      <c r="V23" t="s">
-        <v>209</v>
+      <c r="W23" t="s">
+        <v>277</v>
+      </c>
+      <c r="X23" t="s">
+        <v>275</v>
       </c>
     </row>
-    <row r="24" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>1</v>
       </c>
       <c r="B24" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="C24">
         <v>2017</v>
@@ -2242,39 +2461,45 @@
         <v>114</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="G24">
         <v>7</v>
       </c>
       <c r="H24" t="s">
+        <v>212</v>
+      </c>
+      <c r="I24" t="s">
+        <v>213</v>
+      </c>
+      <c r="J24" t="s">
         <v>214</v>
       </c>
-      <c r="I24" t="s">
+      <c r="K24" t="s">
+        <v>219</v>
+      </c>
+      <c r="M24" t="s">
+        <v>218</v>
+      </c>
+      <c r="Q24" t="s">
+        <v>217</v>
+      </c>
+      <c r="V24" t="s">
         <v>215</v>
       </c>
-      <c r="J24" t="s">
-        <v>216</v>
-      </c>
-      <c r="K24" t="s">
-        <v>221</v>
-      </c>
-      <c r="M24" t="s">
-        <v>220</v>
-      </c>
-      <c r="Q24" t="s">
-        <v>219</v>
-      </c>
-      <c r="V24" t="s">
-        <v>217</v>
+      <c r="W24" t="s">
+        <v>277</v>
+      </c>
+      <c r="X24" t="s">
+        <v>281</v>
       </c>
     </row>
-    <row r="25" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>1</v>
       </c>
       <c r="B25" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="C25">
         <v>2016</v>
@@ -2286,42 +2511,48 @@
         <v>97</v>
       </c>
       <c r="H25" t="s">
+        <v>220</v>
+      </c>
+      <c r="I25" t="s">
+        <v>221</v>
+      </c>
+      <c r="J25" t="s">
+        <v>224</v>
+      </c>
+      <c r="K25" t="s">
+        <v>230</v>
+      </c>
+      <c r="M25" t="s">
+        <v>227</v>
+      </c>
+      <c r="O25" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="P25" t="s">
+        <v>225</v>
+      </c>
+      <c r="S25" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="U25" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="V25" t="s">
         <v>222</v>
       </c>
-      <c r="I25" t="s">
-        <v>223</v>
-      </c>
-      <c r="J25" t="s">
-        <v>226</v>
-      </c>
-      <c r="K25" t="s">
-        <v>232</v>
-      </c>
-      <c r="M25" t="s">
-        <v>229</v>
-      </c>
-      <c r="O25" s="1" t="s">
-        <v>228</v>
-      </c>
-      <c r="P25" t="s">
-        <v>227</v>
-      </c>
-      <c r="S25" s="1" t="s">
-        <v>231</v>
-      </c>
-      <c r="U25" s="1" t="s">
-        <v>230</v>
-      </c>
-      <c r="V25" t="s">
-        <v>224</v>
+      <c r="W25" t="s">
+        <v>267</v>
+      </c>
+      <c r="X25" t="s">
+        <v>262</v>
       </c>
     </row>
-    <row r="26" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>1</v>
       </c>
       <c r="B26" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="C26">
         <v>2015</v>
@@ -2333,31 +2564,37 @@
         <v>114</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="G26">
         <v>27</v>
       </c>
       <c r="H26" t="s">
+        <v>231</v>
+      </c>
+      <c r="I26" t="s">
+        <v>232</v>
+      </c>
+      <c r="J26" t="s">
         <v>233</v>
       </c>
-      <c r="I26" t="s">
+      <c r="K26" t="s">
+        <v>238</v>
+      </c>
+      <c r="M26" t="s">
+        <v>235</v>
+      </c>
+      <c r="Q26" t="s">
+        <v>236</v>
+      </c>
+      <c r="V26" t="s">
         <v>234</v>
       </c>
-      <c r="J26" t="s">
-        <v>235</v>
-      </c>
-      <c r="K26" t="s">
-        <v>240</v>
-      </c>
-      <c r="M26" t="s">
-        <v>237</v>
-      </c>
-      <c r="Q26" t="s">
-        <v>238</v>
-      </c>
-      <c r="V26" t="s">
-        <v>236</v>
+      <c r="W26" t="s">
+        <v>277</v>
+      </c>
+      <c r="X26" t="s">
+        <v>275</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[FEAT] automatically render lab experience
</commit_message>
<xml_diff>
--- a/data/pubs.xlsx
+++ b/data/pubs.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/DoerLBH/Dropbox (Personal)/Git/doerbeta.github.io/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6742B94F-CB43-0742-B02D-E3FC302A38B4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F639E5B-67CF-1B44-8E52-00138CBEE4B3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="47300" yWindow="-3340" windowWidth="28040" windowHeight="17440" xr2:uid="{2388AA68-C25E-CF45-A9DC-089130C49FF2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="282">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="405" uniqueCount="325">
   <si>
     <t>title</t>
   </si>
@@ -71,9 +72,6 @@
     <t>type</t>
   </si>
   <si>
-    <t>miniVox</t>
-  </si>
-  <si>
     <t>P</t>
   </si>
   <si>
@@ -101,9 +99,6 @@
     <t>We proposed a novel AI framework to conduct real-time multi-speaker diarization and recognition without prior registration and pretraining in a fully online learning setting. Our contributions are two-fold. First, we proposed a new benchmark to evaluate the rarely studied fully online speaker diarization problem. We built upon existing datasets of real world utterances to automatically curate MiniVox, an experimental environment which generates infinite configurations of continuous multi-speaker speech stream. Secondly, we considered the practical problem of online learning with episodically revealed rewards and introduced a solution based on semi-supervised and self-supervised learning methods. Lastly, we provided a workable web-based recognition system which interactively handles the cold start problem of new user's addition by transferring representations of old arms to new ones with an extendable contextual bandit. We demonstrated that our proposed method obtained robust performance in the online MiniVox framework.</t>
   </si>
   <si>
-    <t>voiceIDdemo</t>
-  </si>
-  <si>
     <t>VoiceID on the fly: A Speaker Recognition System that Learns from Scratch</t>
   </si>
   <si>
@@ -131,9 +126,6 @@
     <t xml:space="preserve">Adaptive Geo-Topological Independence Criterion   </t>
   </si>
   <si>
-    <t>AGTICnips</t>
-  </si>
-  <si>
     <t>Baihan Lin, Nikolaus Kriegeskorte</t>
   </si>
   <si>
@@ -155,9 +147,6 @@
     <t>Online Learning in Iterated Prisoner's Dilemma to Mimic Human Behavior</t>
   </si>
   <si>
-    <t>dilemmaRLnips</t>
-  </si>
-  <si>
     <t xml:space="preserve">Baihan Lin, Djallel Bouneffouf, Guillermo Cecchi </t>
   </si>
   <si>
@@ -185,9 +174,6 @@
     <t xml:space="preserve">Inspired by the adaptation phenomenon of neuronal firing, we propose the regularity normalization (RN) as an unsupervised attention mechanism (UAM) which computes the statistical regularity in the implicit space of neural networks under the Minimum Description Length (MDL) principle. Treating the neural network optimization process as a partially observable model selection problem, UAM constrained the implicit space by a normalization factor, the universal code length. We compute this universal code incrementally across neural network layers and demonstrated the flexibility to include data priors such as top-down attention and other oracle information. Empirically, our approach outperforms existing normalization methods in tackling limited, imbalanced and non-stationary input distribution in computer vision and reinforcement learning tasks. Lastly, UAM tracks dependency and critical learning stages across layers and recurrent time steps of deep networks. </t>
   </si>
   <si>
-    <t>constrainMDL</t>
-  </si>
-  <si>
     <t>https://arxiv.org/abs/1902.10658</t>
   </si>
   <si>
@@ -203,9 +189,6 @@
     <t>Elongated arm reach after a Pinocchio illusion in Virtual Reality</t>
   </si>
   <si>
-    <t>pinocchio</t>
-  </si>
-  <si>
     <t xml:space="preserve">Mar Gonzalez-Franco, Christopher Berger, Baihan Lin, Bigna Lenggenhager, and Jaron Lanier </t>
   </si>
   <si>
@@ -224,9 +207,6 @@
     <t xml:space="preserve">Baihan Lin, Guillermo Cecchi, Djallel Bouneffouf, Jenna Reinen, Irina Rish </t>
   </si>
   <si>
-    <t>unifiedRL</t>
-  </si>
-  <si>
     <t>lin2020unified.png</t>
   </si>
   <si>
@@ -266,9 +246,6 @@
     <t xml:space="preserve">This paper proposed a new interaction paradigm in the virtual reality (VR) environments, which consists of a virtual mirror or window projected onto a virtual surface, representing the correct perspective geometry of a mirror or window reflecting the real world. This technique can be applied to various videos, live streaming apps, augmented and virtual reality settings to provide an interactive and immersive user experience. To support such a perspective-accurate representation, we implemented computer vision algorithms for feature detection and correspondence matching. To constrain the solutions, we incorporated an automatically tuning scaling factor upon the homography transform matrix such that each image frame follows a smooth transition with the user in sight. The system is a real-time rendering framework where users can engage their real-life presence with the virtual space. </t>
   </si>
   <si>
-    <t>v2r</t>
-  </si>
-  <si>
     <t>video</t>
   </si>
   <si>
@@ -284,9 +261,6 @@
     <t>https://www.youtube.com/watch?v=ZFCMjPiSxIQ</t>
   </si>
   <si>
-    <t>splitQL</t>
-  </si>
-  <si>
     <t>AAMAS 2020</t>
   </si>
   <si>
@@ -329,9 +303,6 @@
     <t>E</t>
   </si>
   <si>
-    <t>splitQLnips</t>
-  </si>
-  <si>
     <t>lin2019reinforce.png</t>
   </si>
   <si>
@@ -350,9 +321,6 @@
     <t>Baihan Lin, Raul Rabadan, Nikolaus Kriegeskorte</t>
   </si>
   <si>
-    <t>scTSAnips</t>
-  </si>
-  <si>
     <t xml:space="preserve">NeurIPS 2019 Workshop on Learning Meaningful Representations of Life (LMRL) </t>
   </si>
   <si>
@@ -380,18 +348,9 @@
     <t>J</t>
   </si>
   <si>
-    <t>andelin2019lack.txt</t>
-  </si>
-  <si>
-    <t>andelin2019lack.pdf</t>
-  </si>
-  <si>
     <t>KDD_MentalRL_slides.pdf</t>
   </si>
   <si>
-    <t>patchjcn</t>
-  </si>
-  <si>
     <t>In albino rats, it has been reported that lateral striate cortex (V1) is highly binocular, and that input from the ipsilateral eye to this region comes through the callosum. In contrast, in Long Evans rats, this region is nearly exclusively dominated by the contralateral eye even though it is richly innervated by the callosum (Laing, Turecek, Takahata, &amp; Olavarria, 2015). We hypothesized that the inability of callosal connections to relay ipsilateral eye input to lateral V1 in Long Evans rats is a consequence of the existence of ocular dominance columns (ODCs), and of callosal patches in register with ipsilateral ODCs in the binocular region of V1 (Laing et al., 2015). We therefore predicted that in albino rats input from both eyes intermix in the binocular region, without segregating into ODCs, and that callosal connections are not patchy. Confirming our predictions, we found that inputs from both eyes, studied with the transneuronal tracer WGA-HRP, are intermixed in the binocular zone of albinos, without segregating into ODCs. Similarly, we found that callosal connections in albino rats are not patchy but instead are distributed homogeneously throughout the callosal region in V1. We propose that these changes allow the transcallosal passage of ipsilateral eye input to lateral striate cortex, increasing its binocularity. Thus, the binocular region in V1 of albino rats includes lateral striate cortex, being therefore about 25% larger in area than the binocular region in Long Evans rats. Our findings provide insight on the role of callosal connections in generating binocular cells.</t>
   </si>
   <si>
@@ -410,18 +369,12 @@
     <t>lin2019modeling.txt</t>
   </si>
   <si>
-    <t>andelin2019lack.png</t>
-  </si>
-  <si>
     <t>lin2019modeling.png</t>
   </si>
   <si>
     <t>https://home.mcleanhospital.org/tips</t>
   </si>
   <si>
-    <t>modelRL</t>
-  </si>
-  <si>
     <t xml:space="preserve">Visualizing Representational Dynamics with Multidimensional Scaling Alignment </t>
   </si>
   <si>
@@ -434,9 +387,6 @@
     <t>https://arxiv.org/abs/1906.09264</t>
   </si>
   <si>
-    <t>RepDynccn</t>
-  </si>
-  <si>
     <t>https://ccneuro.org/2019/Papers/ViewPapers.asp?PaperNum=1424</t>
   </si>
   <si>
@@ -455,9 +405,6 @@
     <t>CCN_MDA_poster.pdf</t>
   </si>
   <si>
-    <t>scTSAismb</t>
-  </si>
-  <si>
     <t>Cliques of single-cell RNA-seq profiles reveal insights into cell ecology during development and differentiation</t>
   </si>
   <si>
@@ -494,9 +441,6 @@
     <t>chen2019self.png</t>
   </si>
   <si>
-    <t>selfAssjacs</t>
-  </si>
-  <si>
     <t>https://pubs.acs.org/toc/jacsat/141/22</t>
   </si>
   <si>
@@ -512,9 +456,6 @@
     <t>Modular self-assembly of biomolecules in two dimensions (2D) is straightforward with DNA but has been difficult to realize with proteins, due to the lack of modular specificity similar to Watson–Crick base pairing. Here we describe a general approach to design 2D arrays using de novo designed pseudosymmetric protein building blocks. A homodimeric helical bundle was reconnected into a monomeric building block, and the surface was redesigned in Rosetta to enable self-assembly into a 2D array in the C12 layer symmetry group. Two out of ten designed arrays assembled to micrometer scale under negative stain electron microscopy, and displayed the designed lattice geometry with assembly size up to 100 nm under atomic force microscopy. The design of 2D arrays with pseudosymmetric building blocks is an important step toward the design of programmable protein self-assembly via pseudosymmetric patterning of orthogonal binding interfaces.</t>
   </si>
   <si>
-    <t>SQLijcai</t>
-  </si>
-  <si>
     <t>Split Q Learning: Reinforcement Learning with Two-Stream Rewards</t>
   </si>
   <si>
@@ -590,9 +531,6 @@
     <t>lin2018adaptive.jpg</t>
   </si>
   <si>
-    <t>ABaCoDEicdm</t>
-  </si>
-  <si>
     <t>Parkinson’s disease digital biomarker discovery with optimized transitions and inferred markov emissions</t>
   </si>
   <si>
@@ -659,9 +597,6 @@
     <t xml:space="preserve">Recently, Zika virus (ZIKV) has been recognized as a significant threat to global public health. The disease was present in large parts of the Americas, the Caribbean, and also the western Pacific area with southern Asia during 2015 and 2016. However, little is known about the factors affecting the transmission of ZIKV. We used Gradient Boosted Regression Tree models to investigate the effects of various potential explanatory variables on the spread of ZIKV, and used current with historical information from a range of sources to assess the risks of future ZIKV outbreaks. Our results indicated that the probability of ZIKV outbreaks increases with vapor pressure, the occurrence of Dengue virus, and population density but decreases as health expenditure, GDP, and numbers of travelers. The predictive results revealed the potential risk countries of ZIKV infection in the Asia-Pacific regions between October 2016 and January 2017. We believe that the high-risk conditions would continue in South Asia and Australia over this period. By integrating information on eco-environmental, social-economical, and ZIKV-related niche factors, this study estimated the probability for locally acquired mosquito-borne ZIKV infections in the Asia-Pacific region and improves the ability to forecast, and possibly even prevent, future outbreaks of ZIKV. </t>
   </si>
   <si>
-    <t>ModelZika</t>
-  </si>
-  <si>
     <t>teng2017model.png</t>
   </si>
   <si>
@@ -683,9 +618,6 @@
     <t xml:space="preserve">Zika virus (ZIKV) infection is an emerging global threat that is suspected to be associated with fetal microcephaly. However, the molecular mechanisms underlying ZIKV disease pathogenesis in humans remain elusive. Here, we investigated the human protein interaction network associated with ZIKV infection using a systemic virology approach, and reconstructed the transcriptional regulatory network to analyze the mechanisms underlying ZIKV-elicited microcephaly pathogenesis. The bioinformatics findings in this study show that P53 is the hub of the genetic regulatory network for ZIKV-related and microcephaly-associated proteins. Importantly, these results imply that the ZIKV capsid protein interacts with mouse double-minute-2 homolog (MDM2), which is involved in the P53-mediated apoptosis pathway, activating the death of infected neural cells. We also found that synthetic mimics of the ZIKV capsid protein induced cell death in vitro and in vivo. This study provides important insight into the relationship between ZIKV infection and brain diseases. </t>
   </si>
   <si>
-    <t>IntegrateZika</t>
-  </si>
-  <si>
     <t>teng2017integrative.pdf</t>
   </si>
   <si>
@@ -704,9 +636,6 @@
     <t xml:space="preserve">What is the effect of sensory deprivation on brain development? Ocular Dominance Columns (ODCs) have been extensively used to study the mechanism of cortical plasticity, despite specific functions of ODCs elusive. Using a combination of transneuronal tracing, in situ hybridization for the immediate early gene Zif268 and electrophysiological recordings, our lab recently showed that the primary visual cortex (V1) in pigmented rats has ODCs correlated with callosal inputs from the opposite hemispheres. Using similar methods, my project aims to understand the effect of monocular deprivation (MD) on the newly discovered system of ODCs in rat visual cortex. I hypothesized that the manipulation of visual input would impact the development and recovery of eye-specific circuitry. By disrupting the visual input permanently or temporarily in early postnatal life, our lab has been able to measure the deleterious effects on map development, critical periods for these effects and potential for recovery. My project used monocular eyelid suture and enucleation to study the effect of MD on the organization of ODCs in pigmented rats. By using our experience-dependent model we expect to elucidate the principles and mechanisms underlying the development of cortical modular architecture in mammals. My result showed a clear shift in Hubel-Wiesel ocular dominance scale in central segment and clear desegregation in ODC in MD rats. I also developed a Java-based software and Matlab protocol to quantify this model. As our hypothesis is supported, our novel model may shed new lights on plasticity research, which can guide future clinical studies on the treatment and prognosis of patients suffering eye defects during early development by either innate or incidental pathological causes. </t>
   </si>
   <si>
-    <t>ODCneurofuture</t>
-  </si>
-  <si>
     <t>NeuroFutures Conference 2016</t>
   </si>
   <si>
@@ -746,9 +675,6 @@
     <t>teng2015systematic.pdf</t>
   </si>
   <si>
-    <t>systemEBOV</t>
-  </si>
-  <si>
     <t>teng2015systematic.png</t>
   </si>
   <si>
@@ -872,13 +798,217 @@
     <t>ML-TM-AM</t>
   </si>
   <si>
-    <t>PDbiomarkerrsg</t>
-  </si>
-  <si>
-    <t>NNmodelijcai</t>
-  </si>
-  <si>
     <t>ML-SB-TM-NS</t>
+  </si>
+  <si>
+    <t>andelin2020influence.png</t>
+  </si>
+  <si>
+    <t>andelin2020influence.txt</t>
+  </si>
+  <si>
+    <t>andelin2020influence.pdf</t>
+  </si>
+  <si>
+    <t>SB-TM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Personalized Genome Group </t>
+  </si>
+  <si>
+    <t>BGI</t>
+  </si>
+  <si>
+    <t>NS-SB-AM-TM</t>
+  </si>
+  <si>
+    <t>State Key Lab of Pathogen &amp; Biosecurity</t>
+  </si>
+  <si>
+    <t>BIME</t>
+  </si>
+  <si>
+    <t>Vision Neuroscience Lab (PI: Olavarria)</t>
+  </si>
+  <si>
+    <t>SB-AM</t>
+  </si>
+  <si>
+    <t>Biophysics Lab of Applied Math (PI: Qian)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Institute for Protein Design (PI: Baker) </t>
+  </si>
+  <si>
+    <t>HCI-ML-TM</t>
+  </si>
+  <si>
+    <t>UbiComp Lab of CSE &amp; EE (PI: Patel)</t>
+  </si>
+  <si>
+    <t>UW</t>
+  </si>
+  <si>
+    <t>SB-ML-TM</t>
+  </si>
+  <si>
+    <t>Comp Bio Lab of CS (PI: Pe’er)</t>
+  </si>
+  <si>
+    <t>SB-ML-GT</t>
+  </si>
+  <si>
+    <t>Math Genomics Lab of DSB (PI: Rabadan)</t>
+  </si>
+  <si>
+    <t>NS-ML-CV-GT-IT</t>
+  </si>
+  <si>
+    <t>Neuro Theory Center (PI: Qian)</t>
+  </si>
+  <si>
+    <t>NS-ML-CV-GT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Visual Inference Lab (PI: Kriegeskorte) </t>
+  </si>
+  <si>
+    <t>Columbia</t>
+  </si>
+  <si>
+    <t>now</t>
+  </si>
+  <si>
+    <t>NS-CV-HCI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EPIC &amp; HCI Groups </t>
+  </si>
+  <si>
+    <t>Microsoft</t>
+  </si>
+  <si>
+    <t>NS-ML-CV-GT-TM</t>
+  </si>
+  <si>
+    <t>CompNeuro &amp; AI Foundations Groups</t>
+  </si>
+  <si>
+    <t>IBM</t>
+  </si>
+  <si>
+    <t>NS-ML-CV-IT-GT-SB-HCI-SP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mostly single-authored </t>
+  </si>
+  <si>
+    <t>my own time</t>
+  </si>
+  <si>
+    <t>on</t>
+  </si>
+  <si>
+    <t>pubs</t>
+  </si>
+  <si>
+    <t>at</t>
+  </si>
+  <si>
+    <t>to</t>
+  </si>
+  <si>
+    <t>from</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>qian</t>
+  </si>
+  <si>
+    <t>rabadan</t>
+  </si>
+  <si>
+    <t>patel</t>
+  </si>
+  <si>
+    <t>uwqian</t>
+  </si>
+  <si>
+    <t>bgi</t>
+  </si>
+  <si>
+    <t>teng2015systematic</t>
+  </si>
+  <si>
+    <t>lin2016odc</t>
+  </si>
+  <si>
+    <t>lin2020speaker</t>
+  </si>
+  <si>
+    <t>lin2020voice</t>
+  </si>
+  <si>
+    <t>lin2018adgtic</t>
+  </si>
+  <si>
+    <t>lin2020online</t>
+  </si>
+  <si>
+    <t>lin2019constraining</t>
+  </si>
+  <si>
+    <t>gonzalez2019enhance</t>
+  </si>
+  <si>
+    <t>lin2020unified</t>
+  </si>
+  <si>
+    <t>lin2020keep</t>
+  </si>
+  <si>
+    <t>lin2020astory</t>
+  </si>
+  <si>
+    <t>lin2019reinforce</t>
+  </si>
+  <si>
+    <t>lin2019what</t>
+  </si>
+  <si>
+    <t>andelin2020influence</t>
+  </si>
+  <si>
+    <t>lin2019modeling</t>
+  </si>
+  <si>
+    <t>lin2019visualize</t>
+  </si>
+  <si>
+    <t>lin2019cliques</t>
+  </si>
+  <si>
+    <t>chen2019self</t>
+  </si>
+  <si>
+    <t>lin2019split</t>
+  </si>
+  <si>
+    <t>lin2018contextual</t>
+  </si>
+  <si>
+    <t>lin2019neural</t>
+  </si>
+  <si>
+    <t>bukkittu2017parkinson</t>
+  </si>
+  <si>
+    <t>teng2017model</t>
+  </si>
+  <si>
+    <t>teng2017integrative</t>
   </si>
 </sst>
 </file>
@@ -1243,8 +1373,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07DC3B69-47EC-374A-9EA9-8E92A8B21FEE}">
   <dimension ref="A1:X26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="X25" sqref="X25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1256,25 +1386,25 @@
   <sheetData>
     <row r="1" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D1" t="s">
-        <v>239</v>
+        <v>214</v>
       </c>
       <c r="E1" t="s">
         <v>11</v>
       </c>
       <c r="F1" t="s">
-        <v>241</v>
+        <v>216</v>
       </c>
       <c r="G1" t="s">
-        <v>240</v>
+        <v>215</v>
       </c>
       <c r="H1" t="s">
         <v>0</v>
@@ -1295,25 +1425,25 @@
         <v>4</v>
       </c>
       <c r="N1" t="s">
-        <v>150</v>
+        <v>132</v>
       </c>
       <c r="O1" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="P1" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="Q1" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="R1" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="S1" t="s">
         <v>5</v>
       </c>
       <c r="T1" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="U1" t="s">
         <v>6</v>
@@ -1322,10 +1452,10 @@
         <v>9</v>
       </c>
       <c r="W1" t="s">
-        <v>253</v>
+        <v>228</v>
       </c>
       <c r="X1" t="s">
-        <v>254</v>
+        <v>229</v>
       </c>
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.2">
@@ -1333,47 +1463,47 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>12</v>
+        <v>303</v>
       </c>
       <c r="D2">
         <v>0</v>
       </c>
       <c r="E2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H2" t="s">
         <v>10</v>
       </c>
       <c r="I2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J2" t="s">
         <v>14</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>15</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="M2" t="s">
         <v>17</v>
       </c>
-      <c r="M2" t="s">
+      <c r="S2" s="1" t="s">
         <v>18</v>
-      </c>
-      <c r="S2" s="1" t="s">
-        <v>19</v>
       </c>
       <c r="T2" s="1"/>
       <c r="U2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="V2" t="s">
         <v>20</v>
       </c>
-      <c r="V2" t="s">
-        <v>21</v>
-      </c>
       <c r="W2" t="s">
-        <v>255</v>
+        <v>230</v>
       </c>
       <c r="X2" t="s">
-        <v>256</v>
+        <v>231</v>
       </c>
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.2">
@@ -1381,7 +1511,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>22</v>
+        <v>304</v>
       </c>
       <c r="C3">
         <v>2020</v>
@@ -1390,40 +1520,40 @@
         <v>10</v>
       </c>
       <c r="E3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="H3" t="s">
+        <v>21</v>
+      </c>
+      <c r="I3" t="s">
+        <v>13</v>
+      </c>
+      <c r="J3" t="s">
         <v>23</v>
       </c>
-      <c r="I3" t="s">
-        <v>14</v>
-      </c>
-      <c r="J3" t="s">
+      <c r="K3" t="s">
         <v>25</v>
       </c>
-      <c r="K3" t="s">
+      <c r="M3" t="s">
+        <v>26</v>
+      </c>
+      <c r="S3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="T3" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="U3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="V3" t="s">
         <v>27</v>
       </c>
-      <c r="M3" t="s">
-        <v>28</v>
-      </c>
-      <c r="S3" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="T3" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="U3" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="V3" t="s">
-        <v>29</v>
-      </c>
       <c r="W3" t="s">
-        <v>255</v>
+        <v>230</v>
       </c>
       <c r="X3" t="s">
-        <v>256</v>
+        <v>231</v>
       </c>
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.2">
@@ -1431,44 +1561,44 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>32</v>
+        <v>305</v>
       </c>
       <c r="D4">
         <v>0</v>
       </c>
       <c r="E4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H4" t="s">
+        <v>29</v>
+      </c>
+      <c r="I4" t="s">
+        <v>30</v>
+      </c>
+      <c r="J4" t="s">
+        <v>14</v>
+      </c>
+      <c r="K4" t="s">
         <v>31</v>
       </c>
-      <c r="I4" t="s">
+      <c r="L4" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="M4" t="s">
         <v>33</v>
       </c>
-      <c r="J4" t="s">
-        <v>15</v>
-      </c>
-      <c r="K4" t="s">
+      <c r="S4" s="1" t="s">
         <v>34</v>
-      </c>
-      <c r="L4" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="M4" t="s">
-        <v>36</v>
-      </c>
-      <c r="S4" s="1" t="s">
-        <v>37</v>
       </c>
       <c r="T4" s="1"/>
       <c r="V4" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="W4" t="s">
-        <v>257</v>
+        <v>232</v>
       </c>
       <c r="X4" t="s">
-        <v>258</v>
+        <v>233</v>
       </c>
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.2">
@@ -1476,50 +1606,50 @@
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>40</v>
+        <v>306</v>
       </c>
       <c r="D5">
         <v>0</v>
       </c>
       <c r="E5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>245</v>
+        <v>220</v>
       </c>
       <c r="G5">
         <v>1</v>
       </c>
       <c r="H5" t="s">
+        <v>36</v>
+      </c>
+      <c r="I5" t="s">
+        <v>37</v>
+      </c>
+      <c r="J5" t="s">
+        <v>14</v>
+      </c>
+      <c r="K5" t="s">
+        <v>38</v>
+      </c>
+      <c r="L5" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="I5" t="s">
+      <c r="M5" t="s">
+        <v>40</v>
+      </c>
+      <c r="S5" s="1" t="s">
         <v>41</v>
-      </c>
-      <c r="J5" t="s">
-        <v>15</v>
-      </c>
-      <c r="K5" t="s">
-        <v>42</v>
-      </c>
-      <c r="L5" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="M5" t="s">
-        <v>44</v>
-      </c>
-      <c r="S5" s="1" t="s">
-        <v>45</v>
       </c>
       <c r="T5" s="1"/>
       <c r="V5" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="W5" t="s">
-        <v>259</v>
+        <v>234</v>
       </c>
       <c r="X5" t="s">
-        <v>263</v>
+        <v>238</v>
       </c>
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.2">
@@ -1527,46 +1657,46 @@
         <v>1</v>
       </c>
       <c r="B6" t="s">
-        <v>50</v>
+        <v>307</v>
       </c>
       <c r="D6">
         <v>0</v>
       </c>
       <c r="E6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H6" t="s">
+        <v>43</v>
+      </c>
+      <c r="I6" t="s">
+        <v>44</v>
+      </c>
+      <c r="J6" t="s">
+        <v>14</v>
+      </c>
+      <c r="K6" t="s">
         <v>47</v>
       </c>
-      <c r="I6" t="s">
+      <c r="L6" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="M6" t="s">
         <v>48</v>
       </c>
-      <c r="J6" t="s">
-        <v>15</v>
-      </c>
-      <c r="K6" t="s">
-        <v>52</v>
-      </c>
-      <c r="L6" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="M6" t="s">
-        <v>53</v>
-      </c>
       <c r="S6" s="1" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="T6" s="1" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="V6" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="W6" t="s">
-        <v>271</v>
+        <v>246</v>
       </c>
       <c r="X6" t="s">
-        <v>260</v>
+        <v>235</v>
       </c>
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.2">
@@ -1574,34 +1704,34 @@
         <v>1</v>
       </c>
       <c r="B7" t="s">
-        <v>56</v>
+        <v>308</v>
       </c>
       <c r="D7">
         <v>-1</v>
       </c>
       <c r="E7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H7" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="I7" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="J7" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="K7" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="V7" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="W7" t="s">
-        <v>261</v>
+        <v>236</v>
       </c>
       <c r="X7" t="s">
-        <v>276</v>
+        <v>251</v>
       </c>
     </row>
     <row r="8" spans="1:24" x14ac:dyDescent="0.2">
@@ -1609,7 +1739,7 @@
         <v>1</v>
       </c>
       <c r="B8" t="s">
-        <v>63</v>
+        <v>309</v>
       </c>
       <c r="C8">
         <v>2020</v>
@@ -1618,49 +1748,49 @@
         <v>8</v>
       </c>
       <c r="E8" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>243</v>
+        <v>218</v>
       </c>
       <c r="G8">
         <v>3</v>
       </c>
       <c r="H8" t="s">
+        <v>55</v>
+      </c>
+      <c r="I8" t="s">
+        <v>56</v>
+      </c>
+      <c r="J8" t="s">
+        <v>64</v>
+      </c>
+      <c r="K8" t="s">
+        <v>57</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="M8" t="s">
+        <v>59</v>
+      </c>
+      <c r="R8" t="s">
+        <v>104</v>
+      </c>
+      <c r="S8" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="T8" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="V8" t="s">
         <v>61</v>
       </c>
-      <c r="I8" t="s">
-        <v>62</v>
-      </c>
-      <c r="J8" t="s">
-        <v>71</v>
-      </c>
-      <c r="K8" t="s">
-        <v>64</v>
-      </c>
-      <c r="L8" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="M8" t="s">
-        <v>66</v>
-      </c>
-      <c r="R8" t="s">
-        <v>117</v>
-      </c>
-      <c r="S8" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="T8" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="V8" t="s">
-        <v>68</v>
-      </c>
       <c r="W8" t="s">
-        <v>259</v>
+        <v>234</v>
       </c>
       <c r="X8" t="s">
-        <v>263</v>
+        <v>238</v>
       </c>
     </row>
     <row r="9" spans="1:24" x14ac:dyDescent="0.2">
@@ -1668,7 +1798,7 @@
         <v>1</v>
       </c>
       <c r="B9" t="s">
-        <v>77</v>
+        <v>310</v>
       </c>
       <c r="C9">
         <v>2020</v>
@@ -1677,38 +1807,38 @@
         <v>7</v>
       </c>
       <c r="E9" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="H9" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="I9" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="J9" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="K9" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="L9" s="1" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="M9" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="S9" s="1" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="T9" s="1"/>
       <c r="V9" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="W9" t="s">
-        <v>255</v>
+        <v>230</v>
       </c>
       <c r="X9" t="s">
-        <v>264</v>
+        <v>239</v>
       </c>
     </row>
     <row r="10" spans="1:24" x14ac:dyDescent="0.2">
@@ -1716,7 +1846,7 @@
         <v>1</v>
       </c>
       <c r="B10" t="s">
-        <v>83</v>
+        <v>311</v>
       </c>
       <c r="C10">
         <v>2020</v>
@@ -1725,49 +1855,49 @@
         <v>5</v>
       </c>
       <c r="E10" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>244</v>
+        <v>219</v>
       </c>
       <c r="G10">
         <v>3</v>
       </c>
       <c r="H10" t="s">
+        <v>76</v>
+      </c>
+      <c r="I10" t="s">
+        <v>56</v>
+      </c>
+      <c r="J10" t="s">
+        <v>75</v>
+      </c>
+      <c r="K10" t="s">
+        <v>77</v>
+      </c>
+      <c r="L10" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="M10" t="s">
+        <v>79</v>
+      </c>
+      <c r="R10" t="s">
+        <v>81</v>
+      </c>
+      <c r="S10" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="T10" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="V10" t="s">
         <v>85</v>
       </c>
-      <c r="I10" t="s">
-        <v>62</v>
-      </c>
-      <c r="J10" t="s">
-        <v>84</v>
-      </c>
-      <c r="K10" t="s">
-        <v>86</v>
-      </c>
-      <c r="L10" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="M10" t="s">
-        <v>88</v>
-      </c>
-      <c r="R10" t="s">
-        <v>90</v>
-      </c>
-      <c r="S10" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="T10" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="V10" t="s">
-        <v>94</v>
-      </c>
       <c r="W10" t="s">
-        <v>259</v>
+        <v>234</v>
       </c>
       <c r="X10" t="s">
-        <v>263</v>
+        <v>238</v>
       </c>
     </row>
     <row r="11" spans="1:24" x14ac:dyDescent="0.2">
@@ -1775,7 +1905,7 @@
         <v>1</v>
       </c>
       <c r="B11" t="s">
-        <v>98</v>
+        <v>312</v>
       </c>
       <c r="C11">
         <v>2019</v>
@@ -1784,40 +1914,40 @@
         <v>12</v>
       </c>
       <c r="E11" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="H11" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="I11" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="J11" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="K11" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
       <c r="L11" s="1" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="M11" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="P11" t="s">
-        <v>101</v>
+        <v>91</v>
       </c>
       <c r="S11" s="1" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="V11" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="W11" t="s">
-        <v>259</v>
+        <v>234</v>
       </c>
       <c r="X11" t="s">
-        <v>263</v>
+        <v>238</v>
       </c>
     </row>
     <row r="12" spans="1:24" x14ac:dyDescent="0.2">
@@ -1825,7 +1955,7 @@
         <v>1</v>
       </c>
       <c r="B12" t="s">
-        <v>105</v>
+        <v>313</v>
       </c>
       <c r="C12">
         <v>2019</v>
@@ -1834,37 +1964,37 @@
         <v>12</v>
       </c>
       <c r="E12" t="s">
+        <v>88</v>
+      </c>
+      <c r="H12" t="s">
+        <v>93</v>
+      </c>
+      <c r="I12" t="s">
+        <v>94</v>
+      </c>
+      <c r="J12" t="s">
+        <v>95</v>
+      </c>
+      <c r="K12" t="s">
         <v>97</v>
       </c>
-      <c r="H12" t="s">
-        <v>103</v>
-      </c>
-      <c r="I12" t="s">
-        <v>104</v>
-      </c>
-      <c r="J12" t="s">
-        <v>106</v>
-      </c>
-      <c r="K12" t="s">
-        <v>108</v>
-      </c>
       <c r="M12" t="s">
-        <v>109</v>
+        <v>98</v>
       </c>
       <c r="P12" t="s">
-        <v>107</v>
+        <v>96</v>
       </c>
       <c r="S12" s="1" t="s">
-        <v>110</v>
+        <v>99</v>
       </c>
       <c r="V12" t="s">
-        <v>111</v>
+        <v>100</v>
       </c>
       <c r="W12" t="s">
-        <v>265</v>
+        <v>240</v>
       </c>
       <c r="X12" t="s">
-        <v>266</v>
+        <v>241</v>
       </c>
     </row>
     <row r="13" spans="1:24" x14ac:dyDescent="0.2">
@@ -1872,7 +2002,7 @@
         <v>1</v>
       </c>
       <c r="B13" t="s">
-        <v>118</v>
+        <v>314</v>
       </c>
       <c r="C13">
         <v>2020</v>
@@ -1881,37 +2011,37 @@
         <v>3</v>
       </c>
       <c r="E13" t="s">
-        <v>114</v>
+        <v>103</v>
       </c>
       <c r="H13" t="s">
-        <v>112</v>
+        <v>101</v>
       </c>
       <c r="I13" t="s">
-        <v>113</v>
+        <v>102</v>
       </c>
       <c r="J13" t="s">
-        <v>252</v>
+        <v>227</v>
       </c>
       <c r="K13" t="s">
-        <v>125</v>
+        <v>255</v>
       </c>
       <c r="M13" t="s">
-        <v>115</v>
+        <v>256</v>
       </c>
       <c r="Q13" t="s">
-        <v>116</v>
+        <v>257</v>
       </c>
       <c r="S13" s="1" t="s">
-        <v>120</v>
+        <v>106</v>
       </c>
       <c r="V13" t="s">
-        <v>119</v>
+        <v>105</v>
       </c>
       <c r="W13" t="s">
-        <v>267</v>
+        <v>242</v>
       </c>
       <c r="X13" t="s">
-        <v>262</v>
+        <v>237</v>
       </c>
     </row>
     <row r="14" spans="1:24" x14ac:dyDescent="0.2">
@@ -1919,7 +2049,7 @@
         <v>1</v>
       </c>
       <c r="B14" t="s">
-        <v>128</v>
+        <v>315</v>
       </c>
       <c r="C14">
         <v>2019</v>
@@ -1928,37 +2058,37 @@
         <v>10</v>
       </c>
       <c r="E14" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="H14" t="s">
-        <v>121</v>
+        <v>107</v>
       </c>
       <c r="I14" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="J14" t="s">
-        <v>122</v>
+        <v>108</v>
       </c>
       <c r="K14" t="s">
-        <v>126</v>
+        <v>111</v>
       </c>
       <c r="M14" t="s">
-        <v>124</v>
+        <v>110</v>
       </c>
       <c r="O14" s="1" t="s">
-        <v>127</v>
+        <v>112</v>
       </c>
       <c r="S14" s="1" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="V14" t="s">
-        <v>123</v>
+        <v>109</v>
       </c>
       <c r="W14" t="s">
-        <v>259</v>
+        <v>234</v>
       </c>
       <c r="X14" t="s">
-        <v>263</v>
+        <v>238</v>
       </c>
     </row>
     <row r="15" spans="1:24" x14ac:dyDescent="0.2">
@@ -1966,7 +2096,7 @@
         <v>1</v>
       </c>
       <c r="B15" t="s">
-        <v>133</v>
+        <v>316</v>
       </c>
       <c r="C15">
         <v>2019</v>
@@ -1975,43 +2105,43 @@
         <v>9</v>
       </c>
       <c r="E15" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="H15" t="s">
-        <v>129</v>
+        <v>113</v>
       </c>
       <c r="I15" t="s">
-        <v>130</v>
+        <v>114</v>
       </c>
       <c r="J15" t="s">
-        <v>131</v>
+        <v>115</v>
       </c>
       <c r="K15" t="s">
-        <v>138</v>
+        <v>121</v>
       </c>
       <c r="L15" s="1" t="s">
-        <v>132</v>
+        <v>116</v>
       </c>
       <c r="M15" t="s">
-        <v>135</v>
+        <v>118</v>
       </c>
       <c r="O15" s="1" t="s">
-        <v>134</v>
+        <v>117</v>
       </c>
       <c r="P15" t="s">
-        <v>139</v>
+        <v>122</v>
       </c>
       <c r="S15" s="1" t="s">
-        <v>136</v>
+        <v>119</v>
       </c>
       <c r="V15" t="s">
-        <v>137</v>
+        <v>120</v>
       </c>
       <c r="W15" t="s">
-        <v>257</v>
+        <v>232</v>
       </c>
       <c r="X15" t="s">
-        <v>268</v>
+        <v>243</v>
       </c>
     </row>
     <row r="16" spans="1:24" x14ac:dyDescent="0.2">
@@ -2019,7 +2149,7 @@
         <v>1</v>
       </c>
       <c r="B16" t="s">
-        <v>140</v>
+        <v>317</v>
       </c>
       <c r="C16">
         <v>2019</v>
@@ -2028,43 +2158,43 @@
         <v>7</v>
       </c>
       <c r="E16" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="H16" t="s">
-        <v>141</v>
+        <v>123</v>
       </c>
       <c r="I16" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="J16" t="s">
-        <v>143</v>
+        <v>125</v>
       </c>
       <c r="K16" t="s">
-        <v>147</v>
+        <v>129</v>
       </c>
       <c r="M16" t="s">
-        <v>144</v>
+        <v>126</v>
       </c>
       <c r="O16" s="1" t="s">
-        <v>142</v>
+        <v>124</v>
       </c>
       <c r="P16" t="s">
-        <v>145</v>
+        <v>127</v>
       </c>
       <c r="R16" t="s">
-        <v>146</v>
+        <v>128</v>
       </c>
       <c r="S16" s="1" t="s">
-        <v>110</v>
+        <v>99</v>
       </c>
       <c r="V16" t="s">
-        <v>111</v>
+        <v>100</v>
       </c>
       <c r="W16" t="s">
-        <v>269</v>
+        <v>244</v>
       </c>
       <c r="X16" t="s">
-        <v>266</v>
+        <v>241</v>
       </c>
     </row>
     <row r="17" spans="1:24" x14ac:dyDescent="0.2">
@@ -2072,7 +2202,7 @@
         <v>1</v>
       </c>
       <c r="B17" t="s">
-        <v>153</v>
+        <v>318</v>
       </c>
       <c r="C17">
         <v>2019</v>
@@ -2081,49 +2211,49 @@
         <v>6</v>
       </c>
       <c r="E17" t="s">
-        <v>114</v>
+        <v>103</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>251</v>
+        <v>226</v>
       </c>
       <c r="G17">
         <v>6</v>
       </c>
       <c r="H17" t="s">
-        <v>148</v>
+        <v>130</v>
       </c>
       <c r="I17" t="s">
-        <v>161</v>
+        <v>141</v>
       </c>
       <c r="J17" t="s">
-        <v>149</v>
+        <v>131</v>
       </c>
       <c r="K17" t="s">
-        <v>152</v>
+        <v>134</v>
       </c>
       <c r="M17" t="s">
-        <v>156</v>
+        <v>137</v>
       </c>
       <c r="N17" t="s">
-        <v>151</v>
+        <v>133</v>
       </c>
       <c r="O17" s="1" t="s">
-        <v>154</v>
+        <v>135</v>
       </c>
       <c r="Q17" t="s">
-        <v>155</v>
+        <v>136</v>
       </c>
       <c r="S17" s="1" t="s">
-        <v>157</v>
+        <v>138</v>
       </c>
       <c r="V17" t="s">
-        <v>158</v>
+        <v>139</v>
       </c>
       <c r="W17" t="s">
-        <v>270</v>
+        <v>245</v>
       </c>
       <c r="X17" t="s">
-        <v>272</v>
+        <v>247</v>
       </c>
     </row>
     <row r="18" spans="1:24" x14ac:dyDescent="0.2">
@@ -2131,7 +2261,7 @@
         <v>1</v>
       </c>
       <c r="B18" t="s">
-        <v>159</v>
+        <v>319</v>
       </c>
       <c r="C18">
         <v>2019</v>
@@ -2140,49 +2270,49 @@
         <v>6</v>
       </c>
       <c r="E18" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>242</v>
+        <v>217</v>
       </c>
       <c r="G18">
         <v>3</v>
       </c>
       <c r="H18" t="s">
-        <v>160</v>
+        <v>140</v>
       </c>
       <c r="I18" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="J18" t="s">
-        <v>162</v>
+        <v>142</v>
       </c>
       <c r="K18" t="s">
-        <v>168</v>
+        <v>148</v>
       </c>
       <c r="L18" s="1" t="s">
-        <v>167</v>
+        <v>147</v>
       </c>
       <c r="M18" t="s">
-        <v>166</v>
+        <v>146</v>
       </c>
       <c r="P18" t="s">
-        <v>165</v>
+        <v>145</v>
       </c>
       <c r="R18" t="s">
-        <v>164</v>
+        <v>144</v>
       </c>
       <c r="S18" s="1" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="V18" t="s">
-        <v>163</v>
+        <v>143</v>
       </c>
       <c r="W18" t="s">
-        <v>259</v>
+        <v>234</v>
       </c>
       <c r="X18" t="s">
-        <v>263</v>
+        <v>238</v>
       </c>
     </row>
     <row r="19" spans="1:24" x14ac:dyDescent="0.2">
@@ -2190,7 +2320,7 @@
         <v>1</v>
       </c>
       <c r="B19" t="s">
-        <v>280</v>
+        <v>321</v>
       </c>
       <c r="C19">
         <v>2019</v>
@@ -2199,43 +2329,43 @@
         <v>6</v>
       </c>
       <c r="E19" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="H19" t="s">
-        <v>169</v>
+        <v>149</v>
       </c>
       <c r="I19" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="J19" t="s">
-        <v>170</v>
+        <v>150</v>
       </c>
       <c r="K19" t="s">
-        <v>176</v>
+        <v>156</v>
       </c>
       <c r="L19" s="1" t="s">
-        <v>171</v>
+        <v>151</v>
       </c>
       <c r="M19" t="s">
-        <v>174</v>
+        <v>154</v>
       </c>
       <c r="P19" t="s">
-        <v>173</v>
+        <v>153</v>
       </c>
       <c r="R19" t="s">
-        <v>172</v>
+        <v>152</v>
       </c>
       <c r="S19" s="1" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="V19" t="s">
-        <v>175</v>
+        <v>155</v>
       </c>
       <c r="W19" t="s">
-        <v>271</v>
+        <v>246</v>
       </c>
       <c r="X19" t="s">
-        <v>260</v>
+        <v>235</v>
       </c>
     </row>
     <row r="20" spans="1:24" x14ac:dyDescent="0.2">
@@ -2243,7 +2373,7 @@
         <v>1</v>
       </c>
       <c r="B20" t="s">
-        <v>185</v>
+        <v>320</v>
       </c>
       <c r="C20">
         <v>2018</v>
@@ -2252,43 +2382,43 @@
         <v>11</v>
       </c>
       <c r="E20" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>250</v>
+        <v>225</v>
       </c>
       <c r="G20">
         <v>10</v>
       </c>
       <c r="H20" t="s">
-        <v>177</v>
+        <v>157</v>
       </c>
       <c r="I20" t="s">
-        <v>178</v>
+        <v>158</v>
       </c>
       <c r="J20" t="s">
-        <v>179</v>
+        <v>159</v>
       </c>
       <c r="K20" t="s">
-        <v>184</v>
+        <v>164</v>
       </c>
       <c r="L20" s="1" t="s">
-        <v>183</v>
+        <v>163</v>
       </c>
       <c r="M20" t="s">
-        <v>182</v>
+        <v>162</v>
       </c>
       <c r="S20" s="1" t="s">
-        <v>181</v>
+        <v>161</v>
       </c>
       <c r="V20" t="s">
-        <v>180</v>
+        <v>160</v>
       </c>
       <c r="W20" t="s">
-        <v>259</v>
+        <v>234</v>
       </c>
       <c r="X20" t="s">
-        <v>273</v>
+        <v>248</v>
       </c>
     </row>
     <row r="21" spans="1:24" x14ac:dyDescent="0.2">
@@ -2296,7 +2426,7 @@
         <v>1</v>
       </c>
       <c r="B21" t="s">
-        <v>279</v>
+        <v>322</v>
       </c>
       <c r="C21">
         <v>2017</v>
@@ -2305,43 +2435,43 @@
         <v>11</v>
       </c>
       <c r="E21" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="H21" t="s">
-        <v>186</v>
+        <v>165</v>
       </c>
       <c r="I21" t="s">
-        <v>187</v>
+        <v>166</v>
       </c>
       <c r="J21" t="s">
-        <v>197</v>
+        <v>176</v>
       </c>
       <c r="K21" t="s">
-        <v>190</v>
+        <v>169</v>
       </c>
       <c r="L21" s="1" t="s">
-        <v>191</v>
+        <v>170</v>
       </c>
       <c r="M21" t="s">
-        <v>189</v>
+        <v>168</v>
       </c>
       <c r="P21" t="s">
-        <v>194</v>
+        <v>173</v>
       </c>
       <c r="R21" t="s">
-        <v>192</v>
+        <v>171</v>
       </c>
       <c r="S21" s="1" t="s">
-        <v>193</v>
+        <v>172</v>
       </c>
       <c r="V21" t="s">
-        <v>188</v>
+        <v>167</v>
       </c>
       <c r="W21" t="s">
-        <v>274</v>
+        <v>249</v>
       </c>
       <c r="X21" t="s">
-        <v>275</v>
+        <v>250</v>
       </c>
     </row>
     <row r="22" spans="1:24" x14ac:dyDescent="0.2">
@@ -2349,7 +2479,7 @@
         <v>1</v>
       </c>
       <c r="B22" t="s">
-        <v>202</v>
+        <v>181</v>
       </c>
       <c r="C22">
         <v>2017</v>
@@ -2358,40 +2488,40 @@
         <v>1</v>
       </c>
       <c r="E22" t="s">
-        <v>114</v>
+        <v>103</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>246</v>
+        <v>221</v>
       </c>
       <c r="G22">
         <v>71</v>
       </c>
       <c r="H22" t="s">
-        <v>195</v>
+        <v>174</v>
       </c>
       <c r="I22" t="s">
-        <v>199</v>
+        <v>178</v>
       </c>
       <c r="J22" t="s">
-        <v>196</v>
+        <v>175</v>
       </c>
       <c r="K22" t="s">
-        <v>203</v>
+        <v>182</v>
       </c>
       <c r="M22" t="s">
-        <v>201</v>
+        <v>180</v>
       </c>
       <c r="Q22" t="s">
-        <v>200</v>
+        <v>179</v>
       </c>
       <c r="V22" t="s">
-        <v>198</v>
+        <v>177</v>
       </c>
       <c r="W22" t="s">
-        <v>277</v>
+        <v>252</v>
       </c>
       <c r="X22" t="s">
-        <v>278</v>
+        <v>253</v>
       </c>
     </row>
     <row r="23" spans="1:24" x14ac:dyDescent="0.2">
@@ -2399,7 +2529,7 @@
         <v>1</v>
       </c>
       <c r="B23" t="s">
-        <v>208</v>
+        <v>323</v>
       </c>
       <c r="C23">
         <v>2017</v>
@@ -2408,40 +2538,40 @@
         <v>5</v>
       </c>
       <c r="E23" t="s">
-        <v>114</v>
+        <v>103</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>248</v>
+        <v>223</v>
       </c>
       <c r="G23">
         <v>15</v>
       </c>
       <c r="H23" t="s">
-        <v>204</v>
+        <v>183</v>
       </c>
       <c r="I23" t="s">
-        <v>206</v>
+        <v>185</v>
       </c>
       <c r="J23" t="s">
-        <v>205</v>
+        <v>184</v>
       </c>
       <c r="K23" t="s">
-        <v>209</v>
+        <v>187</v>
       </c>
       <c r="M23" t="s">
-        <v>211</v>
+        <v>189</v>
       </c>
       <c r="Q23" t="s">
-        <v>210</v>
+        <v>188</v>
       </c>
       <c r="V23" t="s">
-        <v>207</v>
+        <v>186</v>
       </c>
       <c r="W23" t="s">
-        <v>277</v>
+        <v>252</v>
       </c>
       <c r="X23" t="s">
-        <v>275</v>
+        <v>250</v>
       </c>
     </row>
     <row r="24" spans="1:24" x14ac:dyDescent="0.2">
@@ -2449,7 +2579,7 @@
         <v>1</v>
       </c>
       <c r="B24" t="s">
-        <v>216</v>
+        <v>324</v>
       </c>
       <c r="C24">
         <v>2017</v>
@@ -2458,40 +2588,40 @@
         <v>7</v>
       </c>
       <c r="E24" t="s">
-        <v>114</v>
+        <v>103</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>249</v>
+        <v>224</v>
       </c>
       <c r="G24">
         <v>7</v>
       </c>
       <c r="H24" t="s">
-        <v>212</v>
+        <v>190</v>
       </c>
       <c r="I24" t="s">
-        <v>213</v>
+        <v>191</v>
       </c>
       <c r="J24" t="s">
-        <v>214</v>
+        <v>192</v>
       </c>
       <c r="K24" t="s">
-        <v>219</v>
+        <v>196</v>
       </c>
       <c r="M24" t="s">
-        <v>218</v>
+        <v>195</v>
       </c>
       <c r="Q24" t="s">
-        <v>217</v>
+        <v>194</v>
       </c>
       <c r="V24" t="s">
-        <v>215</v>
+        <v>193</v>
       </c>
       <c r="W24" t="s">
-        <v>277</v>
+        <v>252</v>
       </c>
       <c r="X24" t="s">
-        <v>281</v>
+        <v>254</v>
       </c>
     </row>
     <row r="25" spans="1:24" x14ac:dyDescent="0.2">
@@ -2499,7 +2629,7 @@
         <v>1</v>
       </c>
       <c r="B25" t="s">
-        <v>223</v>
+        <v>302</v>
       </c>
       <c r="C25">
         <v>2016</v>
@@ -2508,43 +2638,43 @@
         <v>6</v>
       </c>
       <c r="E25" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="H25" t="s">
-        <v>220</v>
+        <v>197</v>
       </c>
       <c r="I25" t="s">
-        <v>221</v>
+        <v>198</v>
       </c>
       <c r="J25" t="s">
-        <v>224</v>
+        <v>200</v>
       </c>
       <c r="K25" t="s">
-        <v>230</v>
+        <v>206</v>
       </c>
       <c r="M25" t="s">
-        <v>227</v>
+        <v>203</v>
       </c>
       <c r="O25" s="1" t="s">
-        <v>226</v>
+        <v>202</v>
       </c>
       <c r="P25" t="s">
-        <v>225</v>
+        <v>201</v>
       </c>
       <c r="S25" s="1" t="s">
-        <v>229</v>
+        <v>205</v>
       </c>
       <c r="U25" s="1" t="s">
-        <v>228</v>
+        <v>204</v>
       </c>
       <c r="V25" t="s">
-        <v>222</v>
+        <v>199</v>
       </c>
       <c r="W25" t="s">
-        <v>267</v>
+        <v>242</v>
       </c>
       <c r="X25" t="s">
-        <v>262</v>
+        <v>237</v>
       </c>
     </row>
     <row r="26" spans="1:24" x14ac:dyDescent="0.2">
@@ -2552,7 +2682,7 @@
         <v>1</v>
       </c>
       <c r="B26" t="s">
-        <v>237</v>
+        <v>301</v>
       </c>
       <c r="C26">
         <v>2015</v>
@@ -2561,40 +2691,40 @@
         <v>5</v>
       </c>
       <c r="E26" t="s">
-        <v>114</v>
+        <v>103</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>247</v>
+        <v>222</v>
       </c>
       <c r="G26">
         <v>27</v>
       </c>
       <c r="H26" t="s">
-        <v>231</v>
+        <v>207</v>
       </c>
       <c r="I26" t="s">
-        <v>232</v>
+        <v>208</v>
       </c>
       <c r="J26" t="s">
-        <v>233</v>
+        <v>209</v>
       </c>
       <c r="K26" t="s">
-        <v>238</v>
+        <v>213</v>
       </c>
       <c r="M26" t="s">
-        <v>235</v>
+        <v>211</v>
       </c>
       <c r="Q26" t="s">
-        <v>236</v>
+        <v>212</v>
       </c>
       <c r="V26" t="s">
-        <v>234</v>
+        <v>210</v>
       </c>
       <c r="W26" t="s">
-        <v>277</v>
+        <v>252</v>
       </c>
       <c r="X26" t="s">
-        <v>275</v>
+        <v>250</v>
       </c>
     </row>
   </sheetData>
@@ -2657,4 +2787,289 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00934522-8918-5F4D-855B-4574586BDBC0}">
+  <dimension ref="A1:G14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="14.1640625" customWidth="1"/>
+    <col min="4" max="4" width="35.1640625" customWidth="1"/>
+    <col min="5" max="5" width="74" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>294</v>
+      </c>
+      <c r="B1" t="s">
+        <v>293</v>
+      </c>
+      <c r="C1" t="s">
+        <v>292</v>
+      </c>
+      <c r="D1" t="s">
+        <v>228</v>
+      </c>
+      <c r="E1" t="s">
+        <v>291</v>
+      </c>
+      <c r="F1" t="s">
+        <v>290</v>
+      </c>
+      <c r="G1" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>2017</v>
+      </c>
+      <c r="B2" t="s">
+        <v>280</v>
+      </c>
+      <c r="C2" t="s">
+        <v>289</v>
+      </c>
+      <c r="D2" t="s">
+        <v>288</v>
+      </c>
+      <c r="F2" t="s">
+        <v>287</v>
+      </c>
+      <c r="G2" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2017</v>
+      </c>
+      <c r="B3" t="s">
+        <v>280</v>
+      </c>
+      <c r="C3" t="s">
+        <v>286</v>
+      </c>
+      <c r="D3" t="s">
+        <v>285</v>
+      </c>
+      <c r="F3" t="s">
+        <v>284</v>
+      </c>
+      <c r="G3" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>2017</v>
+      </c>
+      <c r="B4">
+        <v>2017</v>
+      </c>
+      <c r="C4" t="s">
+        <v>283</v>
+      </c>
+      <c r="D4" t="s">
+        <v>282</v>
+      </c>
+      <c r="F4" t="s">
+        <v>281</v>
+      </c>
+      <c r="G4" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>2018</v>
+      </c>
+      <c r="B5" t="s">
+        <v>280</v>
+      </c>
+      <c r="C5" t="s">
+        <v>279</v>
+      </c>
+      <c r="D5" t="s">
+        <v>278</v>
+      </c>
+      <c r="F5" t="s">
+        <v>277</v>
+      </c>
+      <c r="G5" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>2018</v>
+      </c>
+      <c r="B6">
+        <v>2019</v>
+      </c>
+      <c r="D6" t="s">
+        <v>276</v>
+      </c>
+      <c r="F6" t="s">
+        <v>275</v>
+      </c>
+      <c r="G6" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>2018</v>
+      </c>
+      <c r="B7">
+        <v>2018</v>
+      </c>
+      <c r="D7" t="s">
+        <v>274</v>
+      </c>
+      <c r="F7" t="s">
+        <v>273</v>
+      </c>
+      <c r="G7" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>2017</v>
+      </c>
+      <c r="B8">
+        <v>2017</v>
+      </c>
+      <c r="D8" t="s">
+        <v>272</v>
+      </c>
+      <c r="F8" t="s">
+        <v>271</v>
+      </c>
+      <c r="G8" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>2017</v>
+      </c>
+      <c r="B9">
+        <v>2017</v>
+      </c>
+      <c r="C9" t="s">
+        <v>270</v>
+      </c>
+      <c r="D9" t="s">
+        <v>269</v>
+      </c>
+      <c r="F9" t="s">
+        <v>268</v>
+      </c>
+      <c r="G9" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>2015</v>
+      </c>
+      <c r="B10">
+        <v>2017</v>
+      </c>
+      <c r="D10" t="s">
+        <v>267</v>
+      </c>
+      <c r="F10" t="s">
+        <v>247</v>
+      </c>
+      <c r="G10" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>2016</v>
+      </c>
+      <c r="B11">
+        <v>2016</v>
+      </c>
+      <c r="D11" t="s">
+        <v>266</v>
+      </c>
+      <c r="F11" t="s">
+        <v>265</v>
+      </c>
+      <c r="G11" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>2014</v>
+      </c>
+      <c r="B12">
+        <v>2016</v>
+      </c>
+      <c r="D12" t="s">
+        <v>264</v>
+      </c>
+      <c r="F12" t="s">
+        <v>237</v>
+      </c>
+      <c r="G12" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>2014</v>
+      </c>
+      <c r="B13">
+        <v>2017</v>
+      </c>
+      <c r="C13" t="s">
+        <v>263</v>
+      </c>
+      <c r="D13" t="s">
+        <v>262</v>
+      </c>
+      <c r="F13" t="s">
+        <v>261</v>
+      </c>
+      <c r="G13" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>2013</v>
+      </c>
+      <c r="B14">
+        <v>2013</v>
+      </c>
+      <c r="C14" t="s">
+        <v>260</v>
+      </c>
+      <c r="D14" t="s">
+        <v>259</v>
+      </c>
+      <c r="F14" t="s">
+        <v>258</v>
+      </c>
+      <c r="G14" t="s">
+        <v>300</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
[DBG] change month sorting rule
</commit_message>
<xml_diff>
--- a/data/pubs.xlsx
+++ b/data/pubs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/DoerLBH/Dropbox (Personal)/Git/doerbeta.github.io/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F639E5B-67CF-1B44-8E52-00138CBEE4B3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6320E010-F85A-1447-B0F0-227D807CE538}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="47300" yWindow="-3340" windowWidth="28040" windowHeight="17440" xr2:uid="{2388AA68-C25E-CF45-A9DC-089130C49FF2}"/>
   </bookViews>
@@ -1374,7 +1374,7 @@
   <dimension ref="A1:X26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
[FEAT] update yt link
</commit_message>
<xml_diff>
--- a/data/pubs.xlsx
+++ b/data/pubs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/DoerLBH/Dropbox (Personal)/Git/doerbeta.github.io/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3612687E-A565-C74F-9608-FFBB548158C8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FA04C48-FBF6-E545-8C4A-DF6D19E97408}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="47640" yWindow="-120" windowWidth="28040" windowHeight="17440" xr2:uid="{2388AA68-C25E-CF45-A9DC-089130C49FF2}"/>
+    <workbookView xWindow="47640" yWindow="-3120" windowWidth="28040" windowHeight="17440" xr2:uid="{2388AA68-C25E-CF45-A9DC-089130C49FF2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -240,9 +240,6 @@
     <t>https://www.youtube.com/watch?v=2d_a1EnIvm4</t>
   </si>
   <si>
-    <t>https://www.youtube.com/watch?v=Y0t-gd7Uz-w</t>
-  </si>
-  <si>
     <t>https://www.youtube.com/watch?v=CQBdQz1bmls</t>
   </si>
   <si>
@@ -1009,6 +1006,9 @@
   </si>
   <si>
     <t>berger2020follow.gif</t>
+  </si>
+  <si>
+    <t>https://youtu.be/QqLnFS5_rCs</t>
   </si>
 </sst>
 </file>
@@ -1374,7 +1374,7 @@
   <dimension ref="A1:X26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M7" sqref="M7"/>
+      <selection activeCell="T4" sqref="T4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1395,16 +1395,16 @@
         <v>24</v>
       </c>
       <c r="D1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E1" t="s">
         <v>11</v>
       </c>
       <c r="F1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="G1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="H1" t="s">
         <v>0</v>
@@ -1425,19 +1425,19 @@
         <v>4</v>
       </c>
       <c r="N1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="O1" t="s">
+        <v>78</v>
+      </c>
+      <c r="P1" t="s">
         <v>79</v>
       </c>
-      <c r="P1" t="s">
-        <v>80</v>
-      </c>
       <c r="Q1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="R1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="S1" t="s">
         <v>5</v>
@@ -1452,10 +1452,10 @@
         <v>9</v>
       </c>
       <c r="W1" t="s">
+        <v>223</v>
+      </c>
+      <c r="X1" t="s">
         <v>224</v>
-      </c>
-      <c r="X1" t="s">
-        <v>225</v>
       </c>
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.2">
@@ -1463,7 +1463,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -1500,10 +1500,10 @@
         <v>20</v>
       </c>
       <c r="W2" t="s">
+        <v>225</v>
+      </c>
+      <c r="X2" t="s">
         <v>226</v>
-      </c>
-      <c r="X2" t="s">
-        <v>227</v>
       </c>
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.2">
@@ -1511,7 +1511,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C3">
         <v>2020</v>
@@ -1541,7 +1541,7 @@
         <v>18</v>
       </c>
       <c r="T3" s="1" t="s">
-        <v>68</v>
+        <v>324</v>
       </c>
       <c r="U3" s="1" t="s">
         <v>19</v>
@@ -1550,10 +1550,10 @@
         <v>27</v>
       </c>
       <c r="W3" t="s">
+        <v>225</v>
+      </c>
+      <c r="X3" t="s">
         <v>226</v>
-      </c>
-      <c r="X3" t="s">
-        <v>227</v>
       </c>
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.2">
@@ -1561,7 +1561,7 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D4">
         <v>0</v>
@@ -1595,10 +1595,10 @@
         <v>35</v>
       </c>
       <c r="W4" t="s">
+        <v>227</v>
+      </c>
+      <c r="X4" t="s">
         <v>228</v>
-      </c>
-      <c r="X4" t="s">
-        <v>229</v>
       </c>
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.2">
@@ -1606,7 +1606,7 @@
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="D5">
         <v>0</v>
@@ -1615,7 +1615,7 @@
         <v>12</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="G5">
         <v>1</v>
@@ -1646,10 +1646,10 @@
         <v>42</v>
       </c>
       <c r="W5" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="X5" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.2">
@@ -1657,7 +1657,7 @@
         <v>1</v>
       </c>
       <c r="B6" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D6">
         <v>0</v>
@@ -1687,16 +1687,16 @@
         <v>49</v>
       </c>
       <c r="T6" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="V6" t="s">
         <v>45</v>
       </c>
       <c r="W6" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="X6" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.2">
@@ -1704,7 +1704,7 @@
         <v>1</v>
       </c>
       <c r="B7" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="D7">
         <v>-1</v>
@@ -1713,25 +1713,25 @@
         <v>12</v>
       </c>
       <c r="H7" t="s">
+        <v>319</v>
+      </c>
+      <c r="I7" t="s">
         <v>320</v>
-      </c>
-      <c r="I7" t="s">
-        <v>321</v>
       </c>
       <c r="J7" t="s">
         <v>50</v>
       </c>
       <c r="K7" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="V7" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="W7" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="X7" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="8" spans="1:24" x14ac:dyDescent="0.2">
@@ -1739,7 +1739,7 @@
         <v>1</v>
       </c>
       <c r="B8" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C8">
         <v>2020</v>
@@ -1751,7 +1751,7 @@
         <v>22</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="G8">
         <v>3</v>
@@ -1775,7 +1775,7 @@
         <v>55</v>
       </c>
       <c r="R8" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="S8" s="1" t="s">
         <v>56</v>
@@ -1787,10 +1787,10 @@
         <v>57</v>
       </c>
       <c r="W8" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="X8" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="9" spans="1:24" x14ac:dyDescent="0.2">
@@ -1798,7 +1798,7 @@
         <v>1</v>
       </c>
       <c r="B9" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C9">
         <v>2020</v>
@@ -1835,10 +1835,10 @@
         <v>65</v>
       </c>
       <c r="W9" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="X9" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="10" spans="1:24" x14ac:dyDescent="0.2">
@@ -1846,7 +1846,7 @@
         <v>1</v>
       </c>
       <c r="B10" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C10">
         <v>2020</v>
@@ -1858,46 +1858,46 @@
         <v>22</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="G10">
         <v>3</v>
       </c>
       <c r="H10" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="I10" t="s">
         <v>52</v>
       </c>
       <c r="J10" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="K10" t="s">
+        <v>72</v>
+      </c>
+      <c r="L10" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="L10" s="1" t="s">
+      <c r="M10" t="s">
         <v>74</v>
       </c>
-      <c r="M10" t="s">
-        <v>75</v>
-      </c>
       <c r="R10" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="S10" s="1" t="s">
         <v>56</v>
       </c>
       <c r="T10" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="V10" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="W10" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="X10" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="11" spans="1:24" x14ac:dyDescent="0.2">
@@ -1905,7 +1905,7 @@
         <v>1</v>
       </c>
       <c r="B11" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C11">
         <v>2019</v>
@@ -1914,40 +1914,40 @@
         <v>12</v>
       </c>
       <c r="E11" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H11" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="I11" t="s">
         <v>52</v>
       </c>
       <c r="J11" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K11" t="s">
+        <v>84</v>
+      </c>
+      <c r="L11" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="M11" t="s">
         <v>85</v>
       </c>
-      <c r="L11" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="M11" t="s">
+      <c r="P11" t="s">
         <v>86</v>
-      </c>
-      <c r="P11" t="s">
-        <v>87</v>
       </c>
       <c r="S11" s="1" t="s">
         <v>56</v>
       </c>
       <c r="V11" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="W11" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="X11" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="12" spans="1:24" x14ac:dyDescent="0.2">
@@ -1955,7 +1955,7 @@
         <v>1</v>
       </c>
       <c r="B12" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C12">
         <v>2019</v>
@@ -1964,37 +1964,37 @@
         <v>12</v>
       </c>
       <c r="E12" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H12" t="s">
+        <v>88</v>
+      </c>
+      <c r="I12" t="s">
         <v>89</v>
       </c>
-      <c r="I12" t="s">
+      <c r="J12" t="s">
         <v>90</v>
       </c>
-      <c r="J12" t="s">
+      <c r="K12" t="s">
+        <v>92</v>
+      </c>
+      <c r="M12" t="s">
+        <v>93</v>
+      </c>
+      <c r="P12" t="s">
         <v>91</v>
       </c>
-      <c r="K12" t="s">
-        <v>93</v>
-      </c>
-      <c r="M12" t="s">
+      <c r="S12" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="P12" t="s">
-        <v>92</v>
-      </c>
-      <c r="S12" s="1" t="s">
+      <c r="V12" t="s">
         <v>95</v>
       </c>
-      <c r="V12" t="s">
-        <v>96</v>
-      </c>
       <c r="W12" t="s">
+        <v>235</v>
+      </c>
+      <c r="X12" t="s">
         <v>236</v>
-      </c>
-      <c r="X12" t="s">
-        <v>237</v>
       </c>
     </row>
     <row r="13" spans="1:24" x14ac:dyDescent="0.2">
@@ -2002,7 +2002,7 @@
         <v>1</v>
       </c>
       <c r="B13" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="C13">
         <v>2020</v>
@@ -2011,37 +2011,37 @@
         <v>3</v>
       </c>
       <c r="E13" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H13" t="s">
+        <v>96</v>
+      </c>
+      <c r="I13" t="s">
         <v>97</v>
       </c>
-      <c r="I13" t="s">
-        <v>98</v>
-      </c>
       <c r="J13" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="K13" t="s">
+        <v>250</v>
+      </c>
+      <c r="M13" t="s">
         <v>251</v>
       </c>
-      <c r="M13" t="s">
+      <c r="Q13" t="s">
         <v>252</v>
       </c>
-      <c r="Q13" t="s">
-        <v>253</v>
-      </c>
       <c r="S13" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="V13" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="W13" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="X13" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="14" spans="1:24" x14ac:dyDescent="0.2">
@@ -2049,7 +2049,7 @@
         <v>1</v>
       </c>
       <c r="B14" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="C14">
         <v>2019</v>
@@ -2058,37 +2058,37 @@
         <v>10</v>
       </c>
       <c r="E14" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H14" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="I14" t="s">
         <v>44</v>
       </c>
       <c r="J14" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="K14" t="s">
+        <v>106</v>
+      </c>
+      <c r="M14" t="s">
+        <v>105</v>
+      </c>
+      <c r="O14" s="1" t="s">
         <v>107</v>
-      </c>
-      <c r="M14" t="s">
-        <v>106</v>
-      </c>
-      <c r="O14" s="1" t="s">
-        <v>108</v>
       </c>
       <c r="S14" s="1" t="s">
         <v>56</v>
       </c>
       <c r="V14" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="W14" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="X14" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="15" spans="1:24" x14ac:dyDescent="0.2">
@@ -2096,7 +2096,7 @@
         <v>1</v>
       </c>
       <c r="B15" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="C15">
         <v>2019</v>
@@ -2108,40 +2108,40 @@
         <v>22</v>
       </c>
       <c r="H15" t="s">
+        <v>108</v>
+      </c>
+      <c r="I15" t="s">
         <v>109</v>
       </c>
-      <c r="I15" t="s">
+      <c r="J15" t="s">
         <v>110</v>
       </c>
-      <c r="J15" t="s">
+      <c r="K15" t="s">
+        <v>116</v>
+      </c>
+      <c r="L15" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="K15" t="s">
+      <c r="M15" t="s">
+        <v>113</v>
+      </c>
+      <c r="O15" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="P15" t="s">
         <v>117</v>
       </c>
-      <c r="L15" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="M15" t="s">
+      <c r="S15" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="O15" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="P15" t="s">
-        <v>118</v>
-      </c>
-      <c r="S15" s="1" t="s">
+      <c r="V15" t="s">
         <v>115</v>
       </c>
-      <c r="V15" t="s">
-        <v>116</v>
-      </c>
       <c r="W15" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="X15" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="16" spans="1:24" x14ac:dyDescent="0.2">
@@ -2149,7 +2149,7 @@
         <v>1</v>
       </c>
       <c r="B16" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C16">
         <v>2019</v>
@@ -2158,43 +2158,43 @@
         <v>7</v>
       </c>
       <c r="E16" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H16" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="I16" t="s">
         <v>44</v>
       </c>
       <c r="J16" t="s">
+        <v>120</v>
+      </c>
+      <c r="K16" t="s">
+        <v>124</v>
+      </c>
+      <c r="M16" t="s">
         <v>121</v>
       </c>
-      <c r="K16" t="s">
-        <v>125</v>
-      </c>
-      <c r="M16" t="s">
+      <c r="O16" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="P16" t="s">
         <v>122</v>
       </c>
-      <c r="O16" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="P16" t="s">
+      <c r="R16" t="s">
         <v>123</v>
       </c>
-      <c r="R16" t="s">
-        <v>124</v>
-      </c>
       <c r="S16" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="V16" t="s">
         <v>95</v>
       </c>
-      <c r="V16" t="s">
-        <v>96</v>
-      </c>
       <c r="W16" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="X16" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="17" spans="1:24" x14ac:dyDescent="0.2">
@@ -2202,7 +2202,7 @@
         <v>1</v>
       </c>
       <c r="B17" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C17">
         <v>2019</v>
@@ -2211,49 +2211,49 @@
         <v>6</v>
       </c>
       <c r="E17" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="G17">
         <v>6</v>
       </c>
       <c r="H17" t="s">
+        <v>125</v>
+      </c>
+      <c r="I17" t="s">
+        <v>136</v>
+      </c>
+      <c r="J17" t="s">
         <v>126</v>
       </c>
-      <c r="I17" t="s">
-        <v>137</v>
-      </c>
-      <c r="J17" t="s">
-        <v>127</v>
-      </c>
       <c r="K17" t="s">
+        <v>129</v>
+      </c>
+      <c r="M17" t="s">
+        <v>132</v>
+      </c>
+      <c r="N17" t="s">
+        <v>128</v>
+      </c>
+      <c r="O17" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="M17" t="s">
+      <c r="Q17" t="s">
+        <v>131</v>
+      </c>
+      <c r="S17" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="N17" t="s">
-        <v>129</v>
-      </c>
-      <c r="O17" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="Q17" t="s">
-        <v>132</v>
-      </c>
-      <c r="S17" s="1" t="s">
+      <c r="V17" t="s">
         <v>134</v>
       </c>
-      <c r="V17" t="s">
-        <v>135</v>
-      </c>
       <c r="W17" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="X17" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="18" spans="1:24" x14ac:dyDescent="0.2">
@@ -2261,7 +2261,7 @@
         <v>1</v>
       </c>
       <c r="B18" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C18">
         <v>2019</v>
@@ -2273,46 +2273,46 @@
         <v>22</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="G18">
         <v>3</v>
       </c>
       <c r="H18" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="I18" t="s">
         <v>37</v>
       </c>
       <c r="J18" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="K18" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="L18" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="M18" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="P18" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="R18" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="S18" s="1" t="s">
         <v>56</v>
       </c>
       <c r="V18" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="W18" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="X18" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="19" spans="1:24" x14ac:dyDescent="0.2">
@@ -2320,7 +2320,7 @@
         <v>1</v>
       </c>
       <c r="B19" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C19">
         <v>2019</v>
@@ -2332,40 +2332,40 @@
         <v>22</v>
       </c>
       <c r="H19" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="I19" t="s">
         <v>44</v>
       </c>
       <c r="J19" t="s">
+        <v>145</v>
+      </c>
+      <c r="K19" t="s">
+        <v>151</v>
+      </c>
+      <c r="L19" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="K19" t="s">
-        <v>152</v>
-      </c>
-      <c r="L19" s="1" t="s">
+      <c r="M19" t="s">
+        <v>149</v>
+      </c>
+      <c r="P19" t="s">
+        <v>148</v>
+      </c>
+      <c r="R19" t="s">
         <v>147</v>
-      </c>
-      <c r="M19" t="s">
-        <v>150</v>
-      </c>
-      <c r="P19" t="s">
-        <v>149</v>
-      </c>
-      <c r="R19" t="s">
-        <v>148</v>
       </c>
       <c r="S19" s="1" t="s">
         <v>49</v>
       </c>
       <c r="V19" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="W19" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="X19" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="20" spans="1:24" x14ac:dyDescent="0.2">
@@ -2373,7 +2373,7 @@
         <v>1</v>
       </c>
       <c r="B20" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="C20">
         <v>2018</v>
@@ -2385,40 +2385,40 @@
         <v>22</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="G20">
         <v>10</v>
       </c>
       <c r="H20" t="s">
+        <v>152</v>
+      </c>
+      <c r="I20" t="s">
         <v>153</v>
       </c>
-      <c r="I20" t="s">
+      <c r="J20" t="s">
         <v>154</v>
       </c>
-      <c r="J20" t="s">
+      <c r="K20" t="s">
+        <v>159</v>
+      </c>
+      <c r="L20" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="M20" t="s">
+        <v>157</v>
+      </c>
+      <c r="S20" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="V20" t="s">
         <v>155</v>
       </c>
-      <c r="K20" t="s">
-        <v>160</v>
-      </c>
-      <c r="L20" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="M20" t="s">
-        <v>158</v>
-      </c>
-      <c r="S20" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="V20" t="s">
-        <v>156</v>
-      </c>
       <c r="W20" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="X20" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="21" spans="1:24" x14ac:dyDescent="0.2">
@@ -2426,7 +2426,7 @@
         <v>1</v>
       </c>
       <c r="B21" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="C21">
         <v>2017</v>
@@ -2435,43 +2435,43 @@
         <v>11</v>
       </c>
       <c r="E21" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H21" t="s">
+        <v>160</v>
+      </c>
+      <c r="I21" t="s">
         <v>161</v>
       </c>
-      <c r="I21" t="s">
+      <c r="J21" t="s">
+        <v>171</v>
+      </c>
+      <c r="K21" t="s">
+        <v>164</v>
+      </c>
+      <c r="L21" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="M21" t="s">
+        <v>163</v>
+      </c>
+      <c r="P21" t="s">
+        <v>168</v>
+      </c>
+      <c r="R21" t="s">
+        <v>166</v>
+      </c>
+      <c r="S21" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="V21" t="s">
         <v>162</v>
       </c>
-      <c r="J21" t="s">
-        <v>172</v>
-      </c>
-      <c r="K21" t="s">
-        <v>165</v>
-      </c>
-      <c r="L21" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="M21" t="s">
-        <v>164</v>
-      </c>
-      <c r="P21" t="s">
-        <v>169</v>
-      </c>
-      <c r="R21" t="s">
-        <v>167</v>
-      </c>
-      <c r="S21" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="V21" t="s">
-        <v>163</v>
-      </c>
       <c r="W21" t="s">
+        <v>244</v>
+      </c>
+      <c r="X21" t="s">
         <v>245</v>
-      </c>
-      <c r="X21" t="s">
-        <v>246</v>
       </c>
     </row>
     <row r="22" spans="1:24" x14ac:dyDescent="0.2">
@@ -2479,7 +2479,7 @@
         <v>1</v>
       </c>
       <c r="B22" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C22">
         <v>2017</v>
@@ -2488,40 +2488,40 @@
         <v>1</v>
       </c>
       <c r="E22" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="G22">
         <v>71</v>
       </c>
       <c r="H22" t="s">
+        <v>169</v>
+      </c>
+      <c r="I22" t="s">
+        <v>173</v>
+      </c>
+      <c r="J22" t="s">
         <v>170</v>
       </c>
-      <c r="I22" t="s">
+      <c r="K22" t="s">
+        <v>177</v>
+      </c>
+      <c r="M22" t="s">
+        <v>175</v>
+      </c>
+      <c r="Q22" t="s">
         <v>174</v>
       </c>
-      <c r="J22" t="s">
-        <v>171</v>
-      </c>
-      <c r="K22" t="s">
-        <v>178</v>
-      </c>
-      <c r="M22" t="s">
-        <v>176</v>
-      </c>
-      <c r="Q22" t="s">
-        <v>175</v>
-      </c>
       <c r="V22" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="W22" t="s">
+        <v>247</v>
+      </c>
+      <c r="X22" t="s">
         <v>248</v>
-      </c>
-      <c r="X22" t="s">
-        <v>249</v>
       </c>
     </row>
     <row r="23" spans="1:24" x14ac:dyDescent="0.2">
@@ -2529,7 +2529,7 @@
         <v>1</v>
       </c>
       <c r="B23" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C23">
         <v>2017</v>
@@ -2538,40 +2538,40 @@
         <v>5</v>
       </c>
       <c r="E23" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="G23">
         <v>15</v>
       </c>
       <c r="H23" t="s">
+        <v>178</v>
+      </c>
+      <c r="I23" t="s">
+        <v>180</v>
+      </c>
+      <c r="J23" t="s">
         <v>179</v>
       </c>
-      <c r="I23" t="s">
+      <c r="K23" t="s">
+        <v>182</v>
+      </c>
+      <c r="M23" t="s">
+        <v>184</v>
+      </c>
+      <c r="Q23" t="s">
+        <v>183</v>
+      </c>
+      <c r="V23" t="s">
         <v>181</v>
       </c>
-      <c r="J23" t="s">
-        <v>180</v>
-      </c>
-      <c r="K23" t="s">
-        <v>183</v>
-      </c>
-      <c r="M23" t="s">
-        <v>185</v>
-      </c>
-      <c r="Q23" t="s">
-        <v>184</v>
-      </c>
-      <c r="V23" t="s">
-        <v>182</v>
-      </c>
       <c r="W23" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="X23" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="24" spans="1:24" x14ac:dyDescent="0.2">
@@ -2579,7 +2579,7 @@
         <v>1</v>
       </c>
       <c r="B24" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="C24">
         <v>2017</v>
@@ -2588,40 +2588,40 @@
         <v>7</v>
       </c>
       <c r="E24" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="G24">
         <v>7</v>
       </c>
       <c r="H24" t="s">
+        <v>185</v>
+      </c>
+      <c r="I24" t="s">
         <v>186</v>
       </c>
-      <c r="I24" t="s">
+      <c r="J24" t="s">
         <v>187</v>
       </c>
-      <c r="J24" t="s">
+      <c r="K24" t="s">
+        <v>191</v>
+      </c>
+      <c r="M24" t="s">
+        <v>190</v>
+      </c>
+      <c r="Q24" t="s">
+        <v>189</v>
+      </c>
+      <c r="V24" t="s">
         <v>188</v>
       </c>
-      <c r="K24" t="s">
-        <v>192</v>
-      </c>
-      <c r="M24" t="s">
-        <v>191</v>
-      </c>
-      <c r="Q24" t="s">
-        <v>190</v>
-      </c>
-      <c r="V24" t="s">
-        <v>189</v>
-      </c>
       <c r="W24" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="X24" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="25" spans="1:24" x14ac:dyDescent="0.2">
@@ -2629,7 +2629,7 @@
         <v>1</v>
       </c>
       <c r="B25" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C25">
         <v>2016</v>
@@ -2638,43 +2638,43 @@
         <v>6</v>
       </c>
       <c r="E25" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H25" t="s">
+        <v>192</v>
+      </c>
+      <c r="I25" t="s">
         <v>193</v>
       </c>
-      <c r="I25" t="s">
+      <c r="J25" t="s">
+        <v>195</v>
+      </c>
+      <c r="K25" t="s">
+        <v>201</v>
+      </c>
+      <c r="M25" t="s">
+        <v>198</v>
+      </c>
+      <c r="O25" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="P25" t="s">
+        <v>196</v>
+      </c>
+      <c r="S25" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="U25" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="V25" t="s">
         <v>194</v>
       </c>
-      <c r="J25" t="s">
-        <v>196</v>
-      </c>
-      <c r="K25" t="s">
-        <v>202</v>
-      </c>
-      <c r="M25" t="s">
-        <v>199</v>
-      </c>
-      <c r="O25" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="P25" t="s">
-        <v>197</v>
-      </c>
-      <c r="S25" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="U25" s="1" t="s">
-        <v>200</v>
-      </c>
-      <c r="V25" t="s">
-        <v>195</v>
-      </c>
       <c r="W25" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="X25" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="26" spans="1:24" x14ac:dyDescent="0.2">
@@ -2682,7 +2682,7 @@
         <v>1</v>
       </c>
       <c r="B26" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C26">
         <v>2015</v>
@@ -2691,40 +2691,40 @@
         <v>5</v>
       </c>
       <c r="E26" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="G26">
         <v>27</v>
       </c>
       <c r="H26" t="s">
+        <v>202</v>
+      </c>
+      <c r="I26" t="s">
         <v>203</v>
       </c>
-      <c r="I26" t="s">
+      <c r="J26" t="s">
         <v>204</v>
       </c>
-      <c r="J26" t="s">
+      <c r="K26" t="s">
+        <v>208</v>
+      </c>
+      <c r="M26" t="s">
+        <v>206</v>
+      </c>
+      <c r="Q26" t="s">
+        <v>207</v>
+      </c>
+      <c r="V26" t="s">
         <v>205</v>
       </c>
-      <c r="K26" t="s">
-        <v>209</v>
-      </c>
-      <c r="M26" t="s">
-        <v>207</v>
-      </c>
-      <c r="Q26" t="s">
-        <v>208</v>
-      </c>
-      <c r="V26" t="s">
-        <v>206</v>
-      </c>
       <c r="W26" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="X26" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
   </sheetData>
@@ -2806,25 +2806,25 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>289</v>
+      </c>
+      <c r="B1" t="s">
+        <v>288</v>
+      </c>
+      <c r="C1" t="s">
+        <v>287</v>
+      </c>
+      <c r="D1" t="s">
+        <v>223</v>
+      </c>
+      <c r="E1" t="s">
+        <v>286</v>
+      </c>
+      <c r="F1" t="s">
+        <v>285</v>
+      </c>
+      <c r="G1" t="s">
         <v>290</v>
-      </c>
-      <c r="B1" t="s">
-        <v>289</v>
-      </c>
-      <c r="C1" t="s">
-        <v>288</v>
-      </c>
-      <c r="D1" t="s">
-        <v>224</v>
-      </c>
-      <c r="E1" t="s">
-        <v>287</v>
-      </c>
-      <c r="F1" t="s">
-        <v>286</v>
-      </c>
-      <c r="G1" t="s">
-        <v>291</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
@@ -2832,19 +2832,19 @@
         <v>2017</v>
       </c>
       <c r="B2" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C2" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="D2" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="F2" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="G2" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
@@ -2852,19 +2852,19 @@
         <v>2017</v>
       </c>
       <c r="B3" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C3" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="D3" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="F3" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="G3" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
@@ -2875,16 +2875,16 @@
         <v>2017</v>
       </c>
       <c r="C4" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="D4" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="F4" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="G4" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
@@ -2892,19 +2892,19 @@
         <v>2018</v>
       </c>
       <c r="B5" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C5" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D5" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="F5" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="G5" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
@@ -2915,13 +2915,13 @@
         <v>2019</v>
       </c>
       <c r="D6" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="F6" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="G6" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
@@ -2932,13 +2932,13 @@
         <v>2018</v>
       </c>
       <c r="D7" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="F7" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="G7" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
@@ -2949,13 +2949,13 @@
         <v>2017</v>
       </c>
       <c r="D8" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="F8" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="G8" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
@@ -2966,16 +2966,16 @@
         <v>2017</v>
       </c>
       <c r="C9" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="D9" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="F9" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="G9" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
@@ -2986,13 +2986,13 @@
         <v>2017</v>
       </c>
       <c r="D10" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="F10" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="G10" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
@@ -3003,13 +3003,13 @@
         <v>2016</v>
       </c>
       <c r="D11" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="F11" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="G11" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
@@ -3020,13 +3020,13 @@
         <v>2016</v>
       </c>
       <c r="D12" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="F12" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="G12" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
@@ -3037,16 +3037,16 @@
         <v>2017</v>
       </c>
       <c r="C13" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D13" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="F13" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="G13" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
@@ -3057,16 +3057,16 @@
         <v>2013</v>
       </c>
       <c r="C14" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D14" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="F14" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="G14" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[DBG] fix area counts
</commit_message>
<xml_diff>
--- a/data/pubs.xlsx
+++ b/data/pubs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/DoerLBH/Dropbox (Personal)/Git/doerbeta.github.io/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18E1E4F7-484F-4840-A184-04F3CA8B26EE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92C0D87F-2376-DB40-A9B5-FD9ADEED6A85}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="9160" yWindow="2860" windowWidth="28040" windowHeight="17440" xr2:uid="{2388AA68-C25E-CF45-A9DC-089130C49FF2}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="335">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="425" uniqueCount="335">
   <si>
     <t>title</t>
   </si>
@@ -1403,8 +1403,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07DC3B69-47EC-374A-9EA9-8E92A8B21FEE}">
   <dimension ref="A1:X28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S8" sqref="S8"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="X3" sqref="X3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1515,6 +1515,9 @@
       </c>
       <c r="W2" t="s">
         <v>223</v>
+      </c>
+      <c r="X2" t="s">
+        <v>241</v>
       </c>
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
[FEAT] fix typo and add link
</commit_message>
<xml_diff>
--- a/data/pubs.xlsx
+++ b/data/pubs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/DoerLBH/Dropbox (Personal)/Git/doerbeta.github.io/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92C0D87F-2376-DB40-A9B5-FD9ADEED6A85}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59C8B996-2994-EB48-A8FF-B96A4ACA4BE3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="9160" yWindow="2860" windowWidth="28040" windowHeight="17440" xr2:uid="{2388AA68-C25E-CF45-A9DC-089130C49FF2}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="425" uniqueCount="335">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="418" uniqueCount="332">
   <si>
     <t>title</t>
   </si>
@@ -1026,19 +1026,10 @@
     <t>We considered a novel practical problem of online learning with episodically revealed rewards, motivated by several real-world applications, where the contexts are nonstationary over different episodes and the reward feedbacks are not always available to the decision making agents. For this online semi-supervised learning setting, we introduced Background Episodic Reward LinUCB (BerlinUCB), a solution that easily incorporates clustering as a self-supervision module to provide useful side information when rewards are not observed. Our experiments on a variety of datasets, both in stationary and nonstationary environments of six different scenarios, demonstrated clear advantages of the proposed approach over the standard contextual bandit. Lastly, we introduced a relevant real-life example where this problem setting is especially useful.</t>
   </si>
   <si>
-    <t>lin2020diabolical</t>
-  </si>
-  <si>
-    <t>Diabolical Games: Reinforcement Learning Environments for Lifelong Learning</t>
-  </si>
-  <si>
-    <t>Baihan</t>
-  </si>
-  <si>
-    <t>lin2020diabolical.png</t>
-  </si>
-  <si>
-    <t>lin2020diabolical.txt</t>
+    <t>https://youtu.be/e8IT1S0HXfY?t=3356</t>
+  </si>
+  <si>
+    <t>interview</t>
   </si>
 </sst>
 </file>
@@ -1401,10 +1392,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07DC3B69-47EC-374A-9EA9-8E92A8B21FEE}">
-  <dimension ref="A1:X28"/>
+  <dimension ref="A1:X27"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="X3" sqref="X3"/>
+      <selection activeCell="S23" sqref="S23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1489,8 +1480,11 @@
       </c>
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
       <c r="B2" t="s">
-        <v>330</v>
+        <v>324</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -1499,19 +1493,25 @@
         <v>12</v>
       </c>
       <c r="H2" t="s">
-        <v>331</v>
+        <v>325</v>
       </c>
       <c r="I2" t="s">
-        <v>332</v>
+        <v>44</v>
       </c>
       <c r="J2" t="s">
         <v>14</v>
       </c>
       <c r="K2" t="s">
-        <v>333</v>
+        <v>326</v>
       </c>
       <c r="M2" t="s">
-        <v>334</v>
+        <v>327</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="V2" t="s">
+        <v>329</v>
       </c>
       <c r="W2" t="s">
         <v>223</v>
@@ -1525,7 +1525,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>324</v>
+        <v>296</v>
       </c>
       <c r="D3">
         <v>0</v>
@@ -1534,31 +1534,38 @@
         <v>12</v>
       </c>
       <c r="H3" t="s">
-        <v>325</v>
+        <v>10</v>
       </c>
       <c r="I3" t="s">
-        <v>44</v>
+        <v>13</v>
       </c>
       <c r="J3" t="s">
         <v>14</v>
       </c>
       <c r="K3" t="s">
-        <v>326</v>
+        <v>15</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>16</v>
       </c>
       <c r="M3" t="s">
-        <v>327</v>
+        <v>17</v>
       </c>
       <c r="S3" s="1" t="s">
-        <v>328</v>
+        <v>18</v>
+      </c>
+      <c r="T3" s="1"/>
+      <c r="U3" s="1" t="s">
+        <v>19</v>
       </c>
       <c r="V3" t="s">
-        <v>329</v>
+        <v>20</v>
       </c>
       <c r="W3" t="s">
         <v>223</v>
       </c>
       <c r="X3" t="s">
-        <v>241</v>
+        <v>224</v>
       </c>
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.2">
@@ -1566,7 +1573,7 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="D4">
         <v>0</v>
@@ -1575,38 +1582,35 @@
         <v>12</v>
       </c>
       <c r="H4" t="s">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="I4" t="s">
-        <v>13</v>
+        <v>30</v>
       </c>
       <c r="J4" t="s">
         <v>14</v>
       </c>
       <c r="K4" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="M4" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="S4" s="1" t="s">
-        <v>18</v>
+        <v>34</v>
       </c>
       <c r="T4" s="1"/>
-      <c r="U4" s="1" t="s">
-        <v>19</v>
-      </c>
       <c r="V4" t="s">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="W4" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="X4" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.2">
@@ -1614,7 +1618,7 @@
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="D5">
         <v>0</v>
@@ -1622,36 +1626,42 @@
       <c r="E5" t="s">
         <v>12</v>
       </c>
+      <c r="F5" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="G5">
+        <v>6</v>
+      </c>
       <c r="H5" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="I5" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="J5" t="s">
         <v>14</v>
       </c>
       <c r="K5" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="M5" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="S5" s="1" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="T5" s="1"/>
       <c r="V5" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="W5" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="X5" t="s">
-        <v>226</v>
+        <v>231</v>
       </c>
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.2">
@@ -1659,7 +1669,7 @@
         <v>1</v>
       </c>
       <c r="B6" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="D6">
         <v>0</v>
@@ -1667,42 +1677,38 @@
       <c r="E6" t="s">
         <v>12</v>
       </c>
-      <c r="F6" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="G6">
-        <v>6</v>
-      </c>
       <c r="H6" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="I6" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="J6" t="s">
         <v>14</v>
       </c>
       <c r="K6" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="M6" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="S6" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="T6" s="1"/>
+        <v>49</v>
+      </c>
+      <c r="T6" s="1" t="s">
+        <v>67</v>
+      </c>
       <c r="V6" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="W6" t="s">
-        <v>227</v>
+        <v>239</v>
       </c>
       <c r="X6" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.2">
@@ -1710,7 +1716,7 @@
         <v>1</v>
       </c>
       <c r="B7" t="s">
-        <v>300</v>
+        <v>320</v>
       </c>
       <c r="D7">
         <v>0</v>
@@ -1719,37 +1725,25 @@
         <v>12</v>
       </c>
       <c r="H7" t="s">
-        <v>43</v>
+        <v>317</v>
       </c>
       <c r="I7" t="s">
-        <v>44</v>
+        <v>318</v>
       </c>
       <c r="J7" t="s">
         <v>14</v>
       </c>
       <c r="K7" t="s">
-        <v>47</v>
-      </c>
-      <c r="L7" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="M7" t="s">
-        <v>48</v>
-      </c>
-      <c r="S7" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="T7" s="1" t="s">
-        <v>67</v>
+        <v>321</v>
       </c>
       <c r="V7" t="s">
-        <v>45</v>
+        <v>319</v>
       </c>
       <c r="W7" t="s">
-        <v>239</v>
+        <v>229</v>
       </c>
       <c r="X7" t="s">
-        <v>228</v>
+        <v>244</v>
       </c>
     </row>
     <row r="8" spans="1:24" x14ac:dyDescent="0.2">
@@ -1757,34 +1751,49 @@
         <v>1</v>
       </c>
       <c r="B8" t="s">
-        <v>320</v>
+        <v>297</v>
+      </c>
+      <c r="C8">
+        <v>2020</v>
       </c>
       <c r="D8">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="E8" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="H8" t="s">
-        <v>317</v>
+        <v>21</v>
       </c>
       <c r="I8" t="s">
-        <v>318</v>
+        <v>13</v>
       </c>
       <c r="J8" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="K8" t="s">
-        <v>321</v>
+        <v>25</v>
+      </c>
+      <c r="M8" t="s">
+        <v>26</v>
+      </c>
+      <c r="S8" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="T8" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="U8" s="1" t="s">
+        <v>19</v>
       </c>
       <c r="V8" t="s">
-        <v>319</v>
+        <v>27</v>
       </c>
       <c r="W8" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="X8" t="s">
-        <v>244</v>
+        <v>224</v>
       </c>
     </row>
     <row r="9" spans="1:24" x14ac:dyDescent="0.2">
@@ -1792,49 +1801,64 @@
         <v>1</v>
       </c>
       <c r="B9" t="s">
-        <v>297</v>
+        <v>301</v>
       </c>
       <c r="C9">
         <v>2020</v>
       </c>
       <c r="D9">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E9" t="s">
         <v>22</v>
       </c>
+      <c r="F9" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="G9">
+        <v>8</v>
+      </c>
       <c r="H9" t="s">
-        <v>21</v>
+        <v>50</v>
       </c>
       <c r="I9" t="s">
-        <v>13</v>
+        <v>51</v>
       </c>
       <c r="J9" t="s">
-        <v>23</v>
+        <v>59</v>
       </c>
       <c r="K9" t="s">
-        <v>25</v>
+        <v>52</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>53</v>
       </c>
       <c r="M9" t="s">
-        <v>26</v>
+        <v>54</v>
+      </c>
+      <c r="N9" t="s">
+        <v>331</v>
+      </c>
+      <c r="O9" s="1" t="s">
+        <v>330</v>
+      </c>
+      <c r="R9" t="s">
+        <v>97</v>
       </c>
       <c r="S9" s="1" t="s">
-        <v>18</v>
+        <v>55</v>
       </c>
       <c r="T9" s="1" t="s">
-        <v>322</v>
-      </c>
-      <c r="U9" s="1" t="s">
-        <v>19</v>
+        <v>323</v>
       </c>
       <c r="V9" t="s">
-        <v>27</v>
+        <v>56</v>
       </c>
       <c r="W9" t="s">
-        <v>223</v>
+        <v>227</v>
       </c>
       <c r="X9" t="s">
-        <v>224</v>
+        <v>231</v>
       </c>
     </row>
     <row r="10" spans="1:24" x14ac:dyDescent="0.2">
@@ -1842,58 +1866,47 @@
         <v>1</v>
       </c>
       <c r="B10" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="C10">
         <v>2020</v>
       </c>
       <c r="D10">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E10" t="s">
         <v>22</v>
       </c>
-      <c r="F10" s="1" t="s">
-        <v>211</v>
-      </c>
-      <c r="G10">
-        <v>8</v>
-      </c>
       <c r="H10" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="I10" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="J10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="K10" t="s">
-        <v>52</v>
+        <v>63</v>
       </c>
       <c r="L10" s="1" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="M10" t="s">
-        <v>54</v>
-      </c>
-      <c r="R10" t="s">
-        <v>97</v>
+        <v>61</v>
       </c>
       <c r="S10" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="T10" s="1" t="s">
-        <v>323</v>
-      </c>
+        <v>62</v>
+      </c>
+      <c r="T10" s="1"/>
       <c r="V10" t="s">
-        <v>56</v>
+        <v>64</v>
       </c>
       <c r="W10" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="X10" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
     </row>
     <row r="11" spans="1:24" x14ac:dyDescent="0.2">
@@ -1901,47 +1914,58 @@
         <v>1</v>
       </c>
       <c r="B11" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="C11">
         <v>2020</v>
       </c>
       <c r="D11">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E11" t="s">
         <v>22</v>
       </c>
+      <c r="F11" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="G11">
+        <v>8</v>
+      </c>
       <c r="H11" t="s">
-        <v>57</v>
+        <v>69</v>
       </c>
       <c r="I11" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="J11" t="s">
-        <v>58</v>
+        <v>68</v>
       </c>
       <c r="K11" t="s">
-        <v>63</v>
+        <v>70</v>
       </c>
       <c r="L11" s="1" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="M11" t="s">
-        <v>61</v>
+        <v>72</v>
+      </c>
+      <c r="R11" t="s">
+        <v>74</v>
       </c>
       <c r="S11" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="T11" s="1"/>
+        <v>55</v>
+      </c>
+      <c r="T11" s="1" t="s">
+        <v>66</v>
+      </c>
       <c r="V11" t="s">
-        <v>64</v>
+        <v>78</v>
       </c>
       <c r="W11" t="s">
-        <v>223</v>
+        <v>227</v>
       </c>
       <c r="X11" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="12" spans="1:24" x14ac:dyDescent="0.2">
@@ -1949,52 +1973,43 @@
         <v>1</v>
       </c>
       <c r="B12" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="C12">
-        <v>2020</v>
+        <v>2019</v>
       </c>
       <c r="D12">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="E12" t="s">
-        <v>22</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>212</v>
-      </c>
-      <c r="G12">
-        <v>8</v>
+        <v>81</v>
       </c>
       <c r="H12" t="s">
-        <v>69</v>
+        <v>79</v>
       </c>
       <c r="I12" t="s">
         <v>51</v>
       </c>
       <c r="J12" t="s">
-        <v>68</v>
+        <v>80</v>
       </c>
       <c r="K12" t="s">
-        <v>70</v>
+        <v>82</v>
       </c>
       <c r="L12" s="1" t="s">
         <v>71</v>
       </c>
       <c r="M12" t="s">
-        <v>72</v>
-      </c>
-      <c r="R12" t="s">
-        <v>74</v>
+        <v>83</v>
+      </c>
+      <c r="P12" t="s">
+        <v>84</v>
       </c>
       <c r="S12" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="T12" s="1" t="s">
-        <v>66</v>
-      </c>
       <c r="V12" t="s">
-        <v>78</v>
+        <v>85</v>
       </c>
       <c r="W12" t="s">
         <v>227</v>
@@ -2008,7 +2023,7 @@
         <v>1</v>
       </c>
       <c r="B13" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="C13">
         <v>2019</v>
@@ -2020,37 +2035,34 @@
         <v>81</v>
       </c>
       <c r="H13" t="s">
-        <v>79</v>
+        <v>86</v>
       </c>
       <c r="I13" t="s">
-        <v>51</v>
+        <v>87</v>
       </c>
       <c r="J13" t="s">
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="K13" t="s">
-        <v>82</v>
-      </c>
-      <c r="L13" s="1" t="s">
-        <v>71</v>
+        <v>90</v>
       </c>
       <c r="M13" t="s">
-        <v>83</v>
+        <v>91</v>
       </c>
       <c r="P13" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="S13" s="1" t="s">
-        <v>55</v>
+        <v>92</v>
       </c>
       <c r="V13" t="s">
-        <v>85</v>
+        <v>93</v>
       </c>
       <c r="W13" t="s">
-        <v>227</v>
+        <v>233</v>
       </c>
       <c r="X13" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
     </row>
     <row r="14" spans="1:24" x14ac:dyDescent="0.2">
@@ -2058,46 +2070,46 @@
         <v>1</v>
       </c>
       <c r="B14" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="C14">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="D14">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="E14" t="s">
-        <v>81</v>
+        <v>96</v>
       </c>
       <c r="H14" t="s">
-        <v>86</v>
+        <v>94</v>
       </c>
       <c r="I14" t="s">
-        <v>87</v>
+        <v>95</v>
       </c>
       <c r="J14" t="s">
-        <v>88</v>
+        <v>220</v>
       </c>
       <c r="K14" t="s">
-        <v>90</v>
+        <v>248</v>
       </c>
       <c r="M14" t="s">
-        <v>91</v>
-      </c>
-      <c r="P14" t="s">
-        <v>89</v>
+        <v>249</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>250</v>
       </c>
       <c r="S14" s="1" t="s">
-        <v>92</v>
+        <v>99</v>
       </c>
       <c r="V14" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="W14" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="X14" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
     </row>
     <row r="15" spans="1:24" x14ac:dyDescent="0.2">
@@ -2105,46 +2117,46 @@
         <v>1</v>
       </c>
       <c r="B15" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="C15">
-        <v>2020</v>
+        <v>2019</v>
       </c>
       <c r="D15">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="E15" t="s">
-        <v>96</v>
+        <v>81</v>
       </c>
       <c r="H15" t="s">
-        <v>94</v>
+        <v>100</v>
       </c>
       <c r="I15" t="s">
-        <v>95</v>
+        <v>44</v>
       </c>
       <c r="J15" t="s">
-        <v>220</v>
+        <v>101</v>
       </c>
       <c r="K15" t="s">
-        <v>248</v>
+        <v>104</v>
       </c>
       <c r="M15" t="s">
-        <v>249</v>
-      </c>
-      <c r="Q15" t="s">
-        <v>250</v>
+        <v>103</v>
+      </c>
+      <c r="O15" s="1" t="s">
+        <v>105</v>
       </c>
       <c r="S15" s="1" t="s">
-        <v>99</v>
+        <v>55</v>
       </c>
       <c r="V15" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="W15" t="s">
-        <v>235</v>
+        <v>227</v>
       </c>
       <c r="X15" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
     </row>
     <row r="16" spans="1:24" x14ac:dyDescent="0.2">
@@ -2152,46 +2164,52 @@
         <v>1</v>
       </c>
       <c r="B16" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="C16">
         <v>2019</v>
       </c>
       <c r="D16">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E16" t="s">
-        <v>81</v>
+        <v>22</v>
       </c>
       <c r="H16" t="s">
-        <v>100</v>
+        <v>106</v>
       </c>
       <c r="I16" t="s">
-        <v>44</v>
+        <v>107</v>
       </c>
       <c r="J16" t="s">
-        <v>101</v>
+        <v>108</v>
       </c>
       <c r="K16" t="s">
-        <v>104</v>
+        <v>114</v>
+      </c>
+      <c r="L16" s="1" t="s">
+        <v>109</v>
       </c>
       <c r="M16" t="s">
-        <v>103</v>
+        <v>111</v>
       </c>
       <c r="O16" s="1" t="s">
-        <v>105</v>
+        <v>110</v>
+      </c>
+      <c r="P16" t="s">
+        <v>115</v>
       </c>
       <c r="S16" s="1" t="s">
-        <v>55</v>
+        <v>112</v>
       </c>
       <c r="V16" t="s">
-        <v>102</v>
+        <v>113</v>
       </c>
       <c r="W16" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="X16" t="s">
-        <v>231</v>
+        <v>236</v>
       </c>
     </row>
     <row r="17" spans="1:24" x14ac:dyDescent="0.2">
@@ -2199,52 +2217,52 @@
         <v>1</v>
       </c>
       <c r="B17" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="C17">
         <v>2019</v>
       </c>
       <c r="D17">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E17" t="s">
-        <v>22</v>
+        <v>81</v>
       </c>
       <c r="H17" t="s">
-        <v>106</v>
+        <v>116</v>
       </c>
       <c r="I17" t="s">
-        <v>107</v>
+        <v>44</v>
       </c>
       <c r="J17" t="s">
-        <v>108</v>
+        <v>118</v>
       </c>
       <c r="K17" t="s">
-        <v>114</v>
-      </c>
-      <c r="L17" s="1" t="s">
-        <v>109</v>
+        <v>122</v>
       </c>
       <c r="M17" t="s">
-        <v>111</v>
+        <v>119</v>
       </c>
       <c r="O17" s="1" t="s">
-        <v>110</v>
+        <v>117</v>
       </c>
       <c r="P17" t="s">
-        <v>115</v>
+        <v>120</v>
+      </c>
+      <c r="R17" t="s">
+        <v>121</v>
       </c>
       <c r="S17" s="1" t="s">
-        <v>112</v>
+        <v>92</v>
       </c>
       <c r="V17" t="s">
-        <v>113</v>
+        <v>93</v>
       </c>
       <c r="W17" t="s">
-        <v>225</v>
+        <v>237</v>
       </c>
       <c r="X17" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
     </row>
     <row r="18" spans="1:24" x14ac:dyDescent="0.2">
@@ -2252,52 +2270,58 @@
         <v>1</v>
       </c>
       <c r="B18" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="C18">
         <v>2019</v>
       </c>
       <c r="D18">
+        <v>6</v>
+      </c>
+      <c r="E18" t="s">
+        <v>96</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="G18">
         <v>7</v>
       </c>
-      <c r="E18" t="s">
-        <v>81</v>
-      </c>
       <c r="H18" t="s">
-        <v>116</v>
+        <v>123</v>
       </c>
       <c r="I18" t="s">
-        <v>44</v>
+        <v>134</v>
       </c>
       <c r="J18" t="s">
-        <v>118</v>
+        <v>124</v>
       </c>
       <c r="K18" t="s">
-        <v>122</v>
+        <v>127</v>
       </c>
       <c r="M18" t="s">
-        <v>119</v>
+        <v>130</v>
+      </c>
+      <c r="N18" t="s">
+        <v>126</v>
       </c>
       <c r="O18" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="P18" t="s">
-        <v>120</v>
-      </c>
-      <c r="R18" t="s">
-        <v>121</v>
+        <v>128</v>
+      </c>
+      <c r="Q18" t="s">
+        <v>129</v>
       </c>
       <c r="S18" s="1" t="s">
-        <v>92</v>
+        <v>131</v>
       </c>
       <c r="V18" t="s">
-        <v>93</v>
+        <v>132</v>
       </c>
       <c r="W18" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="X18" t="s">
-        <v>234</v>
+        <v>240</v>
       </c>
     </row>
     <row r="19" spans="1:24" x14ac:dyDescent="0.2">
@@ -2305,7 +2329,7 @@
         <v>1</v>
       </c>
       <c r="B19" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="C19">
         <v>2019</v>
@@ -2314,49 +2338,49 @@
         <v>6</v>
       </c>
       <c r="E19" t="s">
-        <v>96</v>
+        <v>22</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>219</v>
+        <v>210</v>
       </c>
       <c r="G19">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="H19" t="s">
-        <v>123</v>
+        <v>133</v>
       </c>
       <c r="I19" t="s">
-        <v>134</v>
+        <v>37</v>
       </c>
       <c r="J19" t="s">
-        <v>124</v>
+        <v>135</v>
       </c>
       <c r="K19" t="s">
-        <v>127</v>
+        <v>141</v>
+      </c>
+      <c r="L19" s="1" t="s">
+        <v>140</v>
       </c>
       <c r="M19" t="s">
-        <v>130</v>
-      </c>
-      <c r="N19" t="s">
-        <v>126</v>
-      </c>
-      <c r="O19" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="Q19" t="s">
-        <v>129</v>
+        <v>139</v>
+      </c>
+      <c r="P19" t="s">
+        <v>138</v>
+      </c>
+      <c r="R19" t="s">
+        <v>137</v>
       </c>
       <c r="S19" s="1" t="s">
-        <v>131</v>
+        <v>55</v>
       </c>
       <c r="V19" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="W19" t="s">
-        <v>238</v>
+        <v>227</v>
       </c>
       <c r="X19" t="s">
-        <v>240</v>
+        <v>231</v>
       </c>
     </row>
     <row r="20" spans="1:24" x14ac:dyDescent="0.2">
@@ -2364,7 +2388,7 @@
         <v>1</v>
       </c>
       <c r="B20" t="s">
-        <v>311</v>
+        <v>313</v>
       </c>
       <c r="C20">
         <v>2019</v>
@@ -2375,47 +2399,41 @@
       <c r="E20" t="s">
         <v>22</v>
       </c>
-      <c r="F20" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="G20">
-        <v>4</v>
-      </c>
       <c r="H20" t="s">
-        <v>133</v>
+        <v>142</v>
       </c>
       <c r="I20" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="J20" t="s">
-        <v>135</v>
+        <v>143</v>
       </c>
       <c r="K20" t="s">
-        <v>141</v>
+        <v>149</v>
       </c>
       <c r="L20" s="1" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="M20" t="s">
-        <v>139</v>
+        <v>147</v>
       </c>
       <c r="P20" t="s">
-        <v>138</v>
+        <v>146</v>
       </c>
       <c r="R20" t="s">
-        <v>137</v>
+        <v>145</v>
       </c>
       <c r="S20" s="1" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="V20" t="s">
-        <v>136</v>
+        <v>148</v>
       </c>
       <c r="W20" t="s">
-        <v>227</v>
+        <v>239</v>
       </c>
       <c r="X20" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
     </row>
     <row r="21" spans="1:24" x14ac:dyDescent="0.2">
@@ -2423,52 +2441,52 @@
         <v>1</v>
       </c>
       <c r="B21" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C21">
-        <v>2019</v>
+        <v>2018</v>
       </c>
       <c r="D21">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="E21" t="s">
         <v>22</v>
       </c>
+      <c r="F21" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="G21">
+        <v>17</v>
+      </c>
       <c r="H21" t="s">
-        <v>142</v>
+        <v>150</v>
       </c>
       <c r="I21" t="s">
-        <v>44</v>
+        <v>151</v>
       </c>
       <c r="J21" t="s">
-        <v>143</v>
+        <v>152</v>
       </c>
       <c r="K21" t="s">
-        <v>149</v>
+        <v>157</v>
       </c>
       <c r="L21" s="1" t="s">
-        <v>144</v>
+        <v>156</v>
       </c>
       <c r="M21" t="s">
-        <v>147</v>
-      </c>
-      <c r="P21" t="s">
-        <v>146</v>
-      </c>
-      <c r="R21" t="s">
-        <v>145</v>
+        <v>155</v>
       </c>
       <c r="S21" s="1" t="s">
-        <v>49</v>
+        <v>154</v>
       </c>
       <c r="V21" t="s">
-        <v>148</v>
+        <v>153</v>
       </c>
       <c r="W21" t="s">
-        <v>239</v>
+        <v>227</v>
       </c>
       <c r="X21" t="s">
-        <v>228</v>
+        <v>241</v>
       </c>
     </row>
     <row r="22" spans="1:24" x14ac:dyDescent="0.2">
@@ -2476,52 +2494,52 @@
         <v>1</v>
       </c>
       <c r="B22" t="s">
-        <v>312</v>
+        <v>314</v>
       </c>
       <c r="C22">
-        <v>2018</v>
+        <v>2017</v>
       </c>
       <c r="D22">
         <v>11</v>
       </c>
       <c r="E22" t="s">
-        <v>22</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>218</v>
-      </c>
-      <c r="G22">
-        <v>17</v>
+        <v>81</v>
       </c>
       <c r="H22" t="s">
-        <v>150</v>
+        <v>158</v>
       </c>
       <c r="I22" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="J22" t="s">
-        <v>152</v>
+        <v>169</v>
       </c>
       <c r="K22" t="s">
-        <v>157</v>
+        <v>162</v>
       </c>
       <c r="L22" s="1" t="s">
-        <v>156</v>
+        <v>163</v>
       </c>
       <c r="M22" t="s">
-        <v>155</v>
+        <v>161</v>
+      </c>
+      <c r="P22" t="s">
+        <v>166</v>
+      </c>
+      <c r="R22" t="s">
+        <v>164</v>
       </c>
       <c r="S22" s="1" t="s">
-        <v>154</v>
+        <v>165</v>
       </c>
       <c r="V22" t="s">
-        <v>153</v>
+        <v>160</v>
       </c>
       <c r="W22" t="s">
-        <v>227</v>
+        <v>242</v>
       </c>
       <c r="X22" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
     </row>
     <row r="23" spans="1:24" x14ac:dyDescent="0.2">
@@ -2529,52 +2547,49 @@
         <v>1</v>
       </c>
       <c r="B23" t="s">
-        <v>314</v>
+        <v>174</v>
       </c>
       <c r="C23">
         <v>2017</v>
       </c>
       <c r="D23">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="E23" t="s">
-        <v>81</v>
+        <v>96</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="G23">
+        <v>73</v>
       </c>
       <c r="H23" t="s">
-        <v>158</v>
+        <v>167</v>
       </c>
       <c r="I23" t="s">
-        <v>159</v>
+        <v>171</v>
       </c>
       <c r="J23" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="K23" t="s">
-        <v>162</v>
-      </c>
-      <c r="L23" s="1" t="s">
-        <v>163</v>
+        <v>175</v>
       </c>
       <c r="M23" t="s">
-        <v>161</v>
-      </c>
-      <c r="P23" t="s">
-        <v>166</v>
-      </c>
-      <c r="R23" t="s">
-        <v>164</v>
-      </c>
-      <c r="S23" s="1" t="s">
-        <v>165</v>
+        <v>173</v>
+      </c>
+      <c r="Q23" t="s">
+        <v>172</v>
       </c>
       <c r="V23" t="s">
-        <v>160</v>
+        <v>170</v>
       </c>
       <c r="W23" t="s">
-        <v>242</v>
+        <v>245</v>
       </c>
       <c r="X23" t="s">
-        <v>243</v>
+        <v>246</v>
       </c>
     </row>
     <row r="24" spans="1:24" x14ac:dyDescent="0.2">
@@ -2582,49 +2597,49 @@
         <v>1</v>
       </c>
       <c r="B24" t="s">
-        <v>174</v>
+        <v>315</v>
       </c>
       <c r="C24">
         <v>2017</v>
       </c>
       <c r="D24">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E24" t="s">
         <v>96</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="G24">
-        <v>73</v>
+        <v>15</v>
       </c>
       <c r="H24" t="s">
-        <v>167</v>
+        <v>176</v>
       </c>
       <c r="I24" t="s">
-        <v>171</v>
+        <v>178</v>
       </c>
       <c r="J24" t="s">
-        <v>168</v>
+        <v>177</v>
       </c>
       <c r="K24" t="s">
-        <v>175</v>
+        <v>180</v>
       </c>
       <c r="M24" t="s">
-        <v>173</v>
+        <v>182</v>
       </c>
       <c r="Q24" t="s">
-        <v>172</v>
+        <v>181</v>
       </c>
       <c r="V24" t="s">
-        <v>170</v>
+        <v>179</v>
       </c>
       <c r="W24" t="s">
         <v>245</v>
       </c>
       <c r="X24" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
     </row>
     <row r="25" spans="1:24" x14ac:dyDescent="0.2">
@@ -2632,49 +2647,49 @@
         <v>1</v>
       </c>
       <c r="B25" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="C25">
         <v>2017</v>
       </c>
       <c r="D25">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E25" t="s">
         <v>96</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="G25">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="H25" t="s">
-        <v>176</v>
+        <v>183</v>
       </c>
       <c r="I25" t="s">
-        <v>178</v>
+        <v>184</v>
       </c>
       <c r="J25" t="s">
-        <v>177</v>
+        <v>185</v>
       </c>
       <c r="K25" t="s">
-        <v>180</v>
+        <v>189</v>
       </c>
       <c r="M25" t="s">
-        <v>182</v>
+        <v>188</v>
       </c>
       <c r="Q25" t="s">
-        <v>181</v>
+        <v>187</v>
       </c>
       <c r="V25" t="s">
-        <v>179</v>
+        <v>186</v>
       </c>
       <c r="W25" t="s">
         <v>245</v>
       </c>
       <c r="X25" t="s">
-        <v>243</v>
+        <v>247</v>
       </c>
     </row>
     <row r="26" spans="1:24" x14ac:dyDescent="0.2">
@@ -2682,49 +2697,52 @@
         <v>1</v>
       </c>
       <c r="B26" t="s">
-        <v>316</v>
+        <v>295</v>
       </c>
       <c r="C26">
-        <v>2017</v>
+        <v>2016</v>
       </c>
       <c r="D26">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E26" t="s">
-        <v>96</v>
-      </c>
-      <c r="F26" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="G26">
-        <v>7</v>
+        <v>81</v>
       </c>
       <c r="H26" t="s">
-        <v>183</v>
+        <v>190</v>
       </c>
       <c r="I26" t="s">
-        <v>184</v>
+        <v>191</v>
       </c>
       <c r="J26" t="s">
-        <v>185</v>
+        <v>193</v>
       </c>
       <c r="K26" t="s">
-        <v>189</v>
+        <v>199</v>
       </c>
       <c r="M26" t="s">
-        <v>188</v>
-      </c>
-      <c r="Q26" t="s">
-        <v>187</v>
+        <v>196</v>
+      </c>
+      <c r="O26" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="P26" t="s">
+        <v>194</v>
+      </c>
+      <c r="S26" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="U26" s="1" t="s">
+        <v>197</v>
       </c>
       <c r="V26" t="s">
-        <v>186</v>
+        <v>192</v>
       </c>
       <c r="W26" t="s">
-        <v>245</v>
+        <v>235</v>
       </c>
       <c r="X26" t="s">
-        <v>247</v>
+        <v>230</v>
       </c>
     </row>
     <row r="27" spans="1:24" x14ac:dyDescent="0.2">
@@ -2732,162 +2750,110 @@
         <v>1</v>
       </c>
       <c r="B27" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C27">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="D27">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E27" t="s">
-        <v>81</v>
+        <v>96</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="G27">
+        <v>27</v>
       </c>
       <c r="H27" t="s">
-        <v>190</v>
+        <v>200</v>
       </c>
       <c r="I27" t="s">
-        <v>191</v>
+        <v>201</v>
       </c>
       <c r="J27" t="s">
-        <v>193</v>
+        <v>202</v>
       </c>
       <c r="K27" t="s">
-        <v>199</v>
+        <v>206</v>
       </c>
       <c r="M27" t="s">
-        <v>196</v>
-      </c>
-      <c r="O27" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="P27" t="s">
-        <v>194</v>
-      </c>
-      <c r="S27" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="U27" s="1" t="s">
-        <v>197</v>
+        <v>204</v>
+      </c>
+      <c r="Q27" t="s">
+        <v>205</v>
       </c>
       <c r="V27" t="s">
-        <v>192</v>
+        <v>203</v>
       </c>
       <c r="W27" t="s">
-        <v>235</v>
+        <v>245</v>
       </c>
       <c r="X27" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="28" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A28">
-        <v>1</v>
-      </c>
-      <c r="B28" t="s">
-        <v>294</v>
-      </c>
-      <c r="C28">
-        <v>2015</v>
-      </c>
-      <c r="D28">
-        <v>5</v>
-      </c>
-      <c r="E28" t="s">
-        <v>96</v>
-      </c>
-      <c r="F28" s="1" t="s">
-        <v>215</v>
-      </c>
-      <c r="G28">
-        <v>27</v>
-      </c>
-      <c r="H28" t="s">
-        <v>200</v>
-      </c>
-      <c r="I28" t="s">
-        <v>201</v>
-      </c>
-      <c r="J28" t="s">
-        <v>202</v>
-      </c>
-      <c r="K28" t="s">
-        <v>206</v>
-      </c>
-      <c r="M28" t="s">
-        <v>204</v>
-      </c>
-      <c r="Q28" t="s">
-        <v>205</v>
-      </c>
-      <c r="V28" t="s">
-        <v>203</v>
-      </c>
-      <c r="W28" t="s">
-        <v>245</v>
-      </c>
-      <c r="X28" t="s">
         <v>243</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="L4" r:id="rId1" xr:uid="{5B0F7667-FE37-F34A-AC38-F81CD4469CEC}"/>
-    <hyperlink ref="S4" r:id="rId2" xr:uid="{222EE742-293D-B74F-A089-60E719E67092}"/>
-    <hyperlink ref="U4" r:id="rId3" xr:uid="{8C1EE27C-B9FE-C440-98E9-9894D1FFC943}"/>
-    <hyperlink ref="L5" r:id="rId4" xr:uid="{9B745B18-E099-A548-BC50-85AC8AD0CD6F}"/>
-    <hyperlink ref="S5" r:id="rId5" xr:uid="{89B9F1A5-E13D-0041-B1E9-D4EE7F6CFF7E}"/>
-    <hyperlink ref="L6" r:id="rId6" xr:uid="{F16323BF-11C4-8F4E-885F-F14C9BA59A60}"/>
-    <hyperlink ref="S6" r:id="rId7" xr:uid="{DE895B31-8ACC-7345-8670-4C0CE99341EC}"/>
-    <hyperlink ref="L7" r:id="rId8" xr:uid="{05E1D395-4995-7D42-AF5B-6430E1005FE9}"/>
-    <hyperlink ref="S7" r:id="rId9" xr:uid="{A497B70D-F621-9541-9EAA-E94AA2E164D1}"/>
-    <hyperlink ref="L10" r:id="rId10" xr:uid="{613A6821-00F5-7F46-837A-3CA6FDC4E523}"/>
-    <hyperlink ref="S10" r:id="rId11" xr:uid="{344F2F57-7CF8-A34C-8FA8-B0A5BFE65615}"/>
-    <hyperlink ref="L11" r:id="rId12" xr:uid="{20350B95-5E84-1D49-9321-2E824134522E}"/>
-    <hyperlink ref="S11" r:id="rId13" xr:uid="{C0259699-F280-044F-8C2F-75CDC809FD84}"/>
-    <hyperlink ref="T10" r:id="rId14" xr:uid="{70FB47DE-DBE4-0546-9BCD-A7DF52AECB00}"/>
-    <hyperlink ref="T12" r:id="rId15" xr:uid="{A79A47B4-DE43-6349-A3EA-2892C1288230}"/>
-    <hyperlink ref="T7" r:id="rId16" xr:uid="{456B4AB9-81F0-FC4B-A2DF-C5AF2A00DE6D}"/>
-    <hyperlink ref="L12" r:id="rId17" xr:uid="{833897A9-E560-8142-BC47-F17858FA9587}"/>
-    <hyperlink ref="S12" r:id="rId18" xr:uid="{6BABC62F-6452-374A-9514-5D967BEA7EC4}"/>
-    <hyperlink ref="L13" r:id="rId19" xr:uid="{7CC14624-EB38-7844-9223-227BC8C2F65C}"/>
-    <hyperlink ref="S13" r:id="rId20" xr:uid="{3E24801E-1149-4D4C-9931-4EEF53B59A3F}"/>
-    <hyperlink ref="S14" r:id="rId21" xr:uid="{36139BD1-AD60-9B4A-A83A-7E7EBD23D9F7}"/>
-    <hyperlink ref="S15" r:id="rId22" xr:uid="{D8E5A8B7-67D5-E64D-B384-DF28BF3D10A9}"/>
-    <hyperlink ref="S16" r:id="rId23" xr:uid="{91FE4C01-BD2B-7741-8C46-187B2F04A0FB}"/>
-    <hyperlink ref="O16" r:id="rId24" xr:uid="{1C1760F0-22CF-C942-9D5F-8839D3402DDD}"/>
-    <hyperlink ref="L17" r:id="rId25" xr:uid="{12D9C94F-AA7B-3E4F-92C1-E809F3C7B772}"/>
-    <hyperlink ref="O17" r:id="rId26" xr:uid="{E99AB94B-8663-1D4D-B6E5-085CDE36984C}"/>
-    <hyperlink ref="S17" r:id="rId27" xr:uid="{191EB2D5-CEB1-0E47-A22B-290B87316E6E}"/>
-    <hyperlink ref="O18" r:id="rId28" xr:uid="{D490BAA8-325B-2B4F-B766-A3A8AEB2B15F}"/>
-    <hyperlink ref="S18" r:id="rId29" xr:uid="{226E85E1-79CD-6642-94BB-0DE6E2992790}"/>
-    <hyperlink ref="O19" r:id="rId30" xr:uid="{78392073-9D75-1846-A3FB-7A8A8A6333F5}"/>
-    <hyperlink ref="S19" r:id="rId31" xr:uid="{2ABF4ED3-8972-584E-9CCE-327DB258C8AE}"/>
-    <hyperlink ref="S20" r:id="rId32" xr:uid="{7CD6086F-27FF-6A46-BA5E-9EBD2DE166C5}"/>
-    <hyperlink ref="L20" r:id="rId33" xr:uid="{129E7F4F-4A68-7243-8025-82B79D081A17}"/>
-    <hyperlink ref="L21" r:id="rId34" xr:uid="{6590F57B-9E2C-324A-BD34-47DFBECAA9F1}"/>
-    <hyperlink ref="S21" r:id="rId35" xr:uid="{1F2CAF2C-4852-214E-BAED-9E6AAD908B46}"/>
-    <hyperlink ref="S22" r:id="rId36" xr:uid="{10E1FD9E-EF69-C248-842C-B8BC9CF81646}"/>
-    <hyperlink ref="L22" r:id="rId37" xr:uid="{3DEA9432-1F43-574A-9A31-271BEA5EB7C4}"/>
-    <hyperlink ref="L23" r:id="rId38" xr:uid="{D33D6673-9B0B-2A4D-A737-3CDA039D8EE4}"/>
-    <hyperlink ref="S23" r:id="rId39" xr:uid="{CC678B1F-57AE-AD44-B905-0382A713AEAB}"/>
-    <hyperlink ref="O27" r:id="rId40" xr:uid="{2C092873-109A-7748-9EAA-385EDB9ECBAB}"/>
-    <hyperlink ref="U27" r:id="rId41" xr:uid="{8D9E500F-6DA3-C841-B725-34028D7D31EE}"/>
-    <hyperlink ref="S27" r:id="rId42" xr:uid="{E9C93A7B-6154-904A-8893-573C015F5F8C}"/>
-    <hyperlink ref="F20" r:id="rId43" xr:uid="{1D1FF07E-41E7-4B4E-A01F-103484DDB1C1}"/>
-    <hyperlink ref="F10" r:id="rId44" xr:uid="{A0962830-B0C7-DB48-A943-F141B0A77937}"/>
-    <hyperlink ref="F12" r:id="rId45" xr:uid="{B86DB1F9-01DD-074C-9FA9-B1FE7B87857D}"/>
-    <hyperlink ref="F6" r:id="rId46" xr:uid="{6125CA87-FF6F-C647-ACBC-A090D2F23433}"/>
-    <hyperlink ref="F24" r:id="rId47" xr:uid="{3AF7A6F3-C085-A54F-AA60-B1AAE6D01B3E}"/>
-    <hyperlink ref="F28" r:id="rId48" xr:uid="{CC06C706-794C-774C-8373-B5FC4592F741}"/>
-    <hyperlink ref="F25" r:id="rId49" xr:uid="{5E660FB6-2678-F344-8E15-57526BAD353D}"/>
-    <hyperlink ref="F26" r:id="rId50" xr:uid="{253725BB-7AA3-3A42-9271-200A1FAFAF60}"/>
-    <hyperlink ref="F22" r:id="rId51" xr:uid="{B8C40CFC-E52A-E94D-8A9E-D58EEBE2EB6D}"/>
-    <hyperlink ref="F19" r:id="rId52" xr:uid="{72070C00-E41C-FA43-AE41-20D199D958A9}"/>
-    <hyperlink ref="S3" r:id="rId53" xr:uid="{E401AFF3-1EB2-2B4F-AE3A-5BD6DD40ADAE}"/>
-    <hyperlink ref="U9" r:id="rId54" xr:uid="{E6453EE0-022F-6D40-AF50-86A4E36BC624}"/>
-    <hyperlink ref="S9" r:id="rId55" xr:uid="{E2CC4D2F-7BBF-8C40-8C79-0E95316B80A4}"/>
-    <hyperlink ref="T9" r:id="rId56" xr:uid="{B819CDC6-E8F1-884E-A348-CFAFAA416095}"/>
+    <hyperlink ref="L3" r:id="rId1" xr:uid="{5B0F7667-FE37-F34A-AC38-F81CD4469CEC}"/>
+    <hyperlink ref="S3" r:id="rId2" xr:uid="{222EE742-293D-B74F-A089-60E719E67092}"/>
+    <hyperlink ref="U3" r:id="rId3" xr:uid="{8C1EE27C-B9FE-C440-98E9-9894D1FFC943}"/>
+    <hyperlink ref="L4" r:id="rId4" xr:uid="{9B745B18-E099-A548-BC50-85AC8AD0CD6F}"/>
+    <hyperlink ref="S4" r:id="rId5" xr:uid="{89B9F1A5-E13D-0041-B1E9-D4EE7F6CFF7E}"/>
+    <hyperlink ref="L5" r:id="rId6" xr:uid="{F16323BF-11C4-8F4E-885F-F14C9BA59A60}"/>
+    <hyperlink ref="S5" r:id="rId7" xr:uid="{DE895B31-8ACC-7345-8670-4C0CE99341EC}"/>
+    <hyperlink ref="L6" r:id="rId8" xr:uid="{05E1D395-4995-7D42-AF5B-6430E1005FE9}"/>
+    <hyperlink ref="S6" r:id="rId9" xr:uid="{A497B70D-F621-9541-9EAA-E94AA2E164D1}"/>
+    <hyperlink ref="L9" r:id="rId10" xr:uid="{613A6821-00F5-7F46-837A-3CA6FDC4E523}"/>
+    <hyperlink ref="S9" r:id="rId11" xr:uid="{344F2F57-7CF8-A34C-8FA8-B0A5BFE65615}"/>
+    <hyperlink ref="L10" r:id="rId12" xr:uid="{20350B95-5E84-1D49-9321-2E824134522E}"/>
+    <hyperlink ref="S10" r:id="rId13" xr:uid="{C0259699-F280-044F-8C2F-75CDC809FD84}"/>
+    <hyperlink ref="T9" r:id="rId14" xr:uid="{70FB47DE-DBE4-0546-9BCD-A7DF52AECB00}"/>
+    <hyperlink ref="T11" r:id="rId15" xr:uid="{A79A47B4-DE43-6349-A3EA-2892C1288230}"/>
+    <hyperlink ref="T6" r:id="rId16" xr:uid="{456B4AB9-81F0-FC4B-A2DF-C5AF2A00DE6D}"/>
+    <hyperlink ref="L11" r:id="rId17" xr:uid="{833897A9-E560-8142-BC47-F17858FA9587}"/>
+    <hyperlink ref="S11" r:id="rId18" xr:uid="{6BABC62F-6452-374A-9514-5D967BEA7EC4}"/>
+    <hyperlink ref="L12" r:id="rId19" xr:uid="{7CC14624-EB38-7844-9223-227BC8C2F65C}"/>
+    <hyperlink ref="S12" r:id="rId20" xr:uid="{3E24801E-1149-4D4C-9931-4EEF53B59A3F}"/>
+    <hyperlink ref="S13" r:id="rId21" xr:uid="{36139BD1-AD60-9B4A-A83A-7E7EBD23D9F7}"/>
+    <hyperlink ref="S14" r:id="rId22" xr:uid="{D8E5A8B7-67D5-E64D-B384-DF28BF3D10A9}"/>
+    <hyperlink ref="S15" r:id="rId23" xr:uid="{91FE4C01-BD2B-7741-8C46-187B2F04A0FB}"/>
+    <hyperlink ref="O15" r:id="rId24" xr:uid="{1C1760F0-22CF-C942-9D5F-8839D3402DDD}"/>
+    <hyperlink ref="L16" r:id="rId25" xr:uid="{12D9C94F-AA7B-3E4F-92C1-E809F3C7B772}"/>
+    <hyperlink ref="O16" r:id="rId26" xr:uid="{E99AB94B-8663-1D4D-B6E5-085CDE36984C}"/>
+    <hyperlink ref="S16" r:id="rId27" xr:uid="{191EB2D5-CEB1-0E47-A22B-290B87316E6E}"/>
+    <hyperlink ref="O17" r:id="rId28" xr:uid="{D490BAA8-325B-2B4F-B766-A3A8AEB2B15F}"/>
+    <hyperlink ref="S17" r:id="rId29" xr:uid="{226E85E1-79CD-6642-94BB-0DE6E2992790}"/>
+    <hyperlink ref="O18" r:id="rId30" xr:uid="{78392073-9D75-1846-A3FB-7A8A8A6333F5}"/>
+    <hyperlink ref="S18" r:id="rId31" xr:uid="{2ABF4ED3-8972-584E-9CCE-327DB258C8AE}"/>
+    <hyperlink ref="S19" r:id="rId32" xr:uid="{7CD6086F-27FF-6A46-BA5E-9EBD2DE166C5}"/>
+    <hyperlink ref="L19" r:id="rId33" xr:uid="{129E7F4F-4A68-7243-8025-82B79D081A17}"/>
+    <hyperlink ref="L20" r:id="rId34" xr:uid="{6590F57B-9E2C-324A-BD34-47DFBECAA9F1}"/>
+    <hyperlink ref="S20" r:id="rId35" xr:uid="{1F2CAF2C-4852-214E-BAED-9E6AAD908B46}"/>
+    <hyperlink ref="S21" r:id="rId36" xr:uid="{10E1FD9E-EF69-C248-842C-B8BC9CF81646}"/>
+    <hyperlink ref="L21" r:id="rId37" xr:uid="{3DEA9432-1F43-574A-9A31-271BEA5EB7C4}"/>
+    <hyperlink ref="L22" r:id="rId38" xr:uid="{D33D6673-9B0B-2A4D-A737-3CDA039D8EE4}"/>
+    <hyperlink ref="S22" r:id="rId39" xr:uid="{CC678B1F-57AE-AD44-B905-0382A713AEAB}"/>
+    <hyperlink ref="O26" r:id="rId40" xr:uid="{2C092873-109A-7748-9EAA-385EDB9ECBAB}"/>
+    <hyperlink ref="U26" r:id="rId41" xr:uid="{8D9E500F-6DA3-C841-B725-34028D7D31EE}"/>
+    <hyperlink ref="S26" r:id="rId42" xr:uid="{E9C93A7B-6154-904A-8893-573C015F5F8C}"/>
+    <hyperlink ref="F19" r:id="rId43" xr:uid="{1D1FF07E-41E7-4B4E-A01F-103484DDB1C1}"/>
+    <hyperlink ref="F9" r:id="rId44" xr:uid="{A0962830-B0C7-DB48-A943-F141B0A77937}"/>
+    <hyperlink ref="F11" r:id="rId45" xr:uid="{B86DB1F9-01DD-074C-9FA9-B1FE7B87857D}"/>
+    <hyperlink ref="F5" r:id="rId46" xr:uid="{6125CA87-FF6F-C647-ACBC-A090D2F23433}"/>
+    <hyperlink ref="F23" r:id="rId47" xr:uid="{3AF7A6F3-C085-A54F-AA60-B1AAE6D01B3E}"/>
+    <hyperlink ref="F27" r:id="rId48" xr:uid="{CC06C706-794C-774C-8373-B5FC4592F741}"/>
+    <hyperlink ref="F24" r:id="rId49" xr:uid="{5E660FB6-2678-F344-8E15-57526BAD353D}"/>
+    <hyperlink ref="F25" r:id="rId50" xr:uid="{253725BB-7AA3-3A42-9271-200A1FAFAF60}"/>
+    <hyperlink ref="F21" r:id="rId51" xr:uid="{B8C40CFC-E52A-E94D-8A9E-D58EEBE2EB6D}"/>
+    <hyperlink ref="F18" r:id="rId52" xr:uid="{72070C00-E41C-FA43-AE41-20D199D958A9}"/>
+    <hyperlink ref="S2" r:id="rId53" xr:uid="{E401AFF3-1EB2-2B4F-AE3A-5BD6DD40ADAE}"/>
+    <hyperlink ref="U8" r:id="rId54" xr:uid="{E6453EE0-022F-6D40-AF50-86A4E36BC624}"/>
+    <hyperlink ref="S8" r:id="rId55" xr:uid="{E2CC4D2F-7BBF-8C40-8C79-0E95316B80A4}"/>
+    <hyperlink ref="T8" r:id="rId56" xr:uid="{B819CDC6-E8F1-884E-A348-CFAFAA416095}"/>
+    <hyperlink ref="O9" r:id="rId57" xr:uid="{F7F505AB-D799-E847-B182-FD283FC9648C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
[DBG] change unified model type
</commit_message>
<xml_diff>
--- a/data/pubs.xlsx
+++ b/data/pubs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/DoerLBH/Dropbox (Personal)/Git/doerbeta.github.io/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CE9DDE1-5F93-7045-B061-6597328CFF3E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C96EBE47-B18E-D946-ACB8-4FD7A699376C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="10080" yWindow="2800" windowWidth="28040" windowHeight="17440" xr2:uid="{2388AA68-C25E-CF45-A9DC-089130C49FF2}"/>
   </bookViews>
@@ -1401,7 +1401,7 @@
   <dimension ref="A1:X27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1822,7 +1822,7 @@
         <v>8</v>
       </c>
       <c r="E9" t="s">
-        <v>22</v>
+        <v>79</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>209</v>

</xml_diff>

<commit_message>
[FEAT] add favicon and CV
</commit_message>
<xml_diff>
--- a/data/pubs.xlsx
+++ b/data/pubs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/DoerLBH/Dropbox (Personal)/Git/doerbeta.github.io/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EFCA031-4B47-C34D-BACD-38CFD53BDDD5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A911CF84-CC34-184D-8BAE-2D1564EAC32F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="10080" yWindow="2800" windowWidth="28040" windowHeight="17440" xr2:uid="{2388AA68-C25E-CF45-A9DC-089130C49FF2}"/>
   </bookViews>
@@ -534,9 +534,6 @@
     <t>Dynamic Forecasting of Zika Epidemics Using Google Trends</t>
   </si>
   <si>
-    <t xml:space="preserve">PLoS One </t>
-  </si>
-  <si>
     <t xml:space="preserve">RECOMB/ISCB 2017 Conference on Regulatory &amp; Systems Genomics </t>
   </si>
   <si>
@@ -1039,6 +1036,9 @@
   </si>
   <si>
     <t>https://arxiv.org/abs/2009.08457</t>
+  </si>
+  <si>
+    <t>PLOS ONE</t>
   </si>
 </sst>
 </file>
@@ -1404,7 +1404,7 @@
   <dimension ref="A1:X27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L3" sqref="L3"/>
+      <selection activeCell="J23" sqref="J23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1425,16 +1425,16 @@
         <v>23</v>
       </c>
       <c r="D1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="E1" t="s">
         <v>11</v>
       </c>
       <c r="F1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="G1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="H1" t="s">
         <v>0</v>
@@ -1482,10 +1482,10 @@
         <v>9</v>
       </c>
       <c r="W1" t="s">
+        <v>218</v>
+      </c>
+      <c r="X1" t="s">
         <v>219</v>
-      </c>
-      <c r="X1" t="s">
-        <v>220</v>
       </c>
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.2">
@@ -1493,7 +1493,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="C2">
         <v>2020</v>
@@ -1505,34 +1505,34 @@
         <v>22</v>
       </c>
       <c r="H2" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="I2" t="s">
         <v>42</v>
       </c>
       <c r="J2" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="K2" t="s">
+        <v>323</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="M2" t="s">
         <v>324</v>
       </c>
-      <c r="L2" s="1" t="s">
-        <v>334</v>
-      </c>
-      <c r="M2" t="s">
+      <c r="S2" s="1" t="s">
         <v>325</v>
       </c>
-      <c r="S2" s="1" t="s">
+      <c r="V2" t="s">
         <v>326</v>
       </c>
-      <c r="V2" t="s">
-        <v>327</v>
-      </c>
       <c r="W2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="X2" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.2">
@@ -1540,7 +1540,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="D3">
         <v>0</v>
@@ -1577,10 +1577,10 @@
         <v>20</v>
       </c>
       <c r="W3" t="s">
+        <v>220</v>
+      </c>
+      <c r="X3" t="s">
         <v>221</v>
-      </c>
-      <c r="X3" t="s">
-        <v>222</v>
       </c>
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.2">
@@ -1588,7 +1588,7 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="D4">
         <v>0</v>
@@ -1622,10 +1622,10 @@
         <v>34</v>
       </c>
       <c r="W4" t="s">
+        <v>222</v>
+      </c>
+      <c r="X4" t="s">
         <v>223</v>
-      </c>
-      <c r="X4" t="s">
-        <v>224</v>
       </c>
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.2">
@@ -1633,7 +1633,7 @@
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="D5">
         <v>0</v>
@@ -1642,7 +1642,7 @@
         <v>12</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="G5">
         <v>7</v>
@@ -1673,10 +1673,10 @@
         <v>41</v>
       </c>
       <c r="W5" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="X5" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.2">
@@ -1684,7 +1684,7 @@
         <v>1</v>
       </c>
       <c r="B6" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="D6">
         <v>0</v>
@@ -1693,7 +1693,7 @@
         <v>12</v>
       </c>
       <c r="H6" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="I6" t="s">
         <v>42</v>
@@ -1720,10 +1720,10 @@
         <v>43</v>
       </c>
       <c r="W6" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="X6" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.2">
@@ -1731,7 +1731,7 @@
         <v>1</v>
       </c>
       <c r="B7" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="D7">
         <v>0</v>
@@ -1740,25 +1740,25 @@
         <v>12</v>
       </c>
       <c r="H7" t="s">
+        <v>314</v>
+      </c>
+      <c r="I7" t="s">
         <v>315</v>
-      </c>
-      <c r="I7" t="s">
-        <v>316</v>
       </c>
       <c r="J7" t="s">
         <v>14</v>
       </c>
       <c r="K7" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="V7" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="W7" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="X7" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="8" spans="1:24" x14ac:dyDescent="0.2">
@@ -1766,7 +1766,7 @@
         <v>1</v>
       </c>
       <c r="B8" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C8">
         <v>2020</v>
@@ -1784,13 +1784,13 @@
         <v>13</v>
       </c>
       <c r="J8" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="K8" t="s">
         <v>24</v>
       </c>
       <c r="L8" s="1" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="M8" t="s">
         <v>25</v>
@@ -1799,7 +1799,7 @@
         <v>18</v>
       </c>
       <c r="T8" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="U8" s="1" t="s">
         <v>19</v>
@@ -1808,10 +1808,10 @@
         <v>26</v>
       </c>
       <c r="W8" t="s">
+        <v>220</v>
+      </c>
+      <c r="X8" t="s">
         <v>221</v>
-      </c>
-      <c r="X8" t="s">
-        <v>222</v>
       </c>
     </row>
     <row r="9" spans="1:24" x14ac:dyDescent="0.2">
@@ -1819,7 +1819,7 @@
         <v>1</v>
       </c>
       <c r="B9" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C9">
         <v>2020</v>
@@ -1831,7 +1831,7 @@
         <v>79</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="G9">
         <v>8</v>
@@ -1855,10 +1855,10 @@
         <v>52</v>
       </c>
       <c r="N9" t="s">
+        <v>327</v>
+      </c>
+      <c r="O9" s="1" t="s">
         <v>328</v>
-      </c>
-      <c r="O9" s="1" t="s">
-        <v>329</v>
       </c>
       <c r="R9" t="s">
         <v>95</v>
@@ -1867,16 +1867,16 @@
         <v>53</v>
       </c>
       <c r="T9" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="V9" t="s">
         <v>54</v>
       </c>
       <c r="W9" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="X9" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="10" spans="1:24" x14ac:dyDescent="0.2">
@@ -1884,7 +1884,7 @@
         <v>1</v>
       </c>
       <c r="B10" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C10">
         <v>2020</v>
@@ -1921,10 +1921,10 @@
         <v>62</v>
       </c>
       <c r="W10" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="X10" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="11" spans="1:24" x14ac:dyDescent="0.2">
@@ -1932,7 +1932,7 @@
         <v>1</v>
       </c>
       <c r="B11" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C11">
         <v>2020</v>
@@ -1944,7 +1944,7 @@
         <v>22</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="G11">
         <v>9</v>
@@ -1980,10 +1980,10 @@
         <v>76</v>
       </c>
       <c r="W11" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="X11" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="12" spans="1:24" x14ac:dyDescent="0.2">
@@ -1991,7 +1991,7 @@
         <v>1</v>
       </c>
       <c r="B12" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C12">
         <v>2019</v>
@@ -2030,10 +2030,10 @@
         <v>83</v>
       </c>
       <c r="W12" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="X12" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="13" spans="1:24" x14ac:dyDescent="0.2">
@@ -2041,7 +2041,7 @@
         <v>1</v>
       </c>
       <c r="B13" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C13">
         <v>2019</v>
@@ -2077,10 +2077,10 @@
         <v>91</v>
       </c>
       <c r="W13" t="s">
+        <v>230</v>
+      </c>
+      <c r="X13" t="s">
         <v>231</v>
-      </c>
-      <c r="X13" t="s">
-        <v>232</v>
       </c>
     </row>
     <row r="14" spans="1:24" x14ac:dyDescent="0.2">
@@ -2088,7 +2088,7 @@
         <v>1</v>
       </c>
       <c r="B14" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C14">
         <v>2020</v>
@@ -2106,16 +2106,16 @@
         <v>93</v>
       </c>
       <c r="J14" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="K14" t="s">
+        <v>245</v>
+      </c>
+      <c r="M14" t="s">
         <v>246</v>
       </c>
-      <c r="M14" t="s">
+      <c r="Q14" t="s">
         <v>247</v>
-      </c>
-      <c r="Q14" t="s">
-        <v>248</v>
       </c>
       <c r="S14" s="1" t="s">
         <v>97</v>
@@ -2124,10 +2124,10 @@
         <v>96</v>
       </c>
       <c r="W14" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="X14" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="15" spans="1:24" x14ac:dyDescent="0.2">
@@ -2135,7 +2135,7 @@
         <v>1</v>
       </c>
       <c r="B15" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C15">
         <v>2019</v>
@@ -2171,10 +2171,10 @@
         <v>100</v>
       </c>
       <c r="W15" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="X15" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="16" spans="1:24" x14ac:dyDescent="0.2">
@@ -2182,7 +2182,7 @@
         <v>1</v>
       </c>
       <c r="B16" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C16">
         <v>2019</v>
@@ -2224,10 +2224,10 @@
         <v>111</v>
       </c>
       <c r="W16" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="X16" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="17" spans="1:24" x14ac:dyDescent="0.2">
@@ -2235,7 +2235,7 @@
         <v>1</v>
       </c>
       <c r="B17" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C17">
         <v>2019</v>
@@ -2277,10 +2277,10 @@
         <v>91</v>
       </c>
       <c r="W17" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="X17" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="18" spans="1:24" x14ac:dyDescent="0.2">
@@ -2288,7 +2288,7 @@
         <v>1</v>
       </c>
       <c r="B18" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C18">
         <v>2019</v>
@@ -2300,7 +2300,7 @@
         <v>94</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="G18">
         <v>9</v>
@@ -2336,10 +2336,10 @@
         <v>130</v>
       </c>
       <c r="W18" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="X18" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="19" spans="1:24" x14ac:dyDescent="0.2">
@@ -2347,7 +2347,7 @@
         <v>1</v>
       </c>
       <c r="B19" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="C19">
         <v>2019</v>
@@ -2359,7 +2359,7 @@
         <v>22</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="G19">
         <v>5</v>
@@ -2395,10 +2395,10 @@
         <v>134</v>
       </c>
       <c r="W19" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="X19" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="20" spans="1:24" x14ac:dyDescent="0.2">
@@ -2406,7 +2406,7 @@
         <v>1</v>
       </c>
       <c r="B20" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="C20">
         <v>2019</v>
@@ -2448,10 +2448,10 @@
         <v>146</v>
       </c>
       <c r="W20" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="X20" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="21" spans="1:24" x14ac:dyDescent="0.2">
@@ -2459,7 +2459,7 @@
         <v>1</v>
       </c>
       <c r="B21" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="C21">
         <v>2018</v>
@@ -2471,7 +2471,7 @@
         <v>22</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="G21">
         <v>18</v>
@@ -2501,10 +2501,10 @@
         <v>151</v>
       </c>
       <c r="W21" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="X21" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="22" spans="1:24" x14ac:dyDescent="0.2">
@@ -2512,7 +2512,7 @@
         <v>1</v>
       </c>
       <c r="B22" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C22">
         <v>2017</v>
@@ -2530,7 +2530,7 @@
         <v>157</v>
       </c>
       <c r="J22" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="K22" t="s">
         <v>160</v>
@@ -2554,10 +2554,10 @@
         <v>158</v>
       </c>
       <c r="W22" t="s">
+        <v>239</v>
+      </c>
+      <c r="X22" t="s">
         <v>240</v>
-      </c>
-      <c r="X22" t="s">
-        <v>241</v>
       </c>
     </row>
     <row r="23" spans="1:24" x14ac:dyDescent="0.2">
@@ -2565,7 +2565,7 @@
         <v>1</v>
       </c>
       <c r="B23" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C23">
         <v>2017</v>
@@ -2577,7 +2577,7 @@
         <v>94</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="G23">
         <v>74</v>
@@ -2586,28 +2586,28 @@
         <v>165</v>
       </c>
       <c r="I23" t="s">
+        <v>168</v>
+      </c>
+      <c r="J23" t="s">
+        <v>334</v>
+      </c>
+      <c r="K23" t="s">
+        <v>172</v>
+      </c>
+      <c r="M23" t="s">
+        <v>170</v>
+      </c>
+      <c r="Q23" t="s">
         <v>169</v>
       </c>
-      <c r="J23" t="s">
-        <v>166</v>
-      </c>
-      <c r="K23" t="s">
-        <v>173</v>
-      </c>
-      <c r="M23" t="s">
-        <v>171</v>
-      </c>
-      <c r="Q23" t="s">
-        <v>170</v>
-      </c>
       <c r="V23" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="W23" t="s">
+        <v>242</v>
+      </c>
+      <c r="X23" t="s">
         <v>243</v>
-      </c>
-      <c r="X23" t="s">
-        <v>244</v>
       </c>
     </row>
     <row r="24" spans="1:24" x14ac:dyDescent="0.2">
@@ -2615,7 +2615,7 @@
         <v>1</v>
       </c>
       <c r="B24" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C24">
         <v>2017</v>
@@ -2627,37 +2627,37 @@
         <v>94</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="G24">
         <v>15</v>
       </c>
       <c r="H24" t="s">
+        <v>173</v>
+      </c>
+      <c r="I24" t="s">
+        <v>175</v>
+      </c>
+      <c r="J24" t="s">
         <v>174</v>
       </c>
-      <c r="I24" t="s">
+      <c r="K24" t="s">
+        <v>177</v>
+      </c>
+      <c r="M24" t="s">
+        <v>179</v>
+      </c>
+      <c r="Q24" t="s">
+        <v>178</v>
+      </c>
+      <c r="V24" t="s">
         <v>176</v>
       </c>
-      <c r="J24" t="s">
-        <v>175</v>
-      </c>
-      <c r="K24" t="s">
-        <v>178</v>
-      </c>
-      <c r="M24" t="s">
-        <v>180</v>
-      </c>
-      <c r="Q24" t="s">
-        <v>179</v>
-      </c>
-      <c r="V24" t="s">
-        <v>177</v>
-      </c>
       <c r="W24" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="X24" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="25" spans="1:24" x14ac:dyDescent="0.2">
@@ -2665,7 +2665,7 @@
         <v>1</v>
       </c>
       <c r="B25" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C25">
         <v>2017</v>
@@ -2677,37 +2677,37 @@
         <v>94</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="G25">
         <v>8</v>
       </c>
       <c r="H25" t="s">
+        <v>180</v>
+      </c>
+      <c r="I25" t="s">
         <v>181</v>
       </c>
-      <c r="I25" t="s">
+      <c r="J25" t="s">
         <v>182</v>
       </c>
-      <c r="J25" t="s">
+      <c r="K25" t="s">
+        <v>186</v>
+      </c>
+      <c r="M25" t="s">
+        <v>185</v>
+      </c>
+      <c r="Q25" t="s">
+        <v>184</v>
+      </c>
+      <c r="V25" t="s">
         <v>183</v>
       </c>
-      <c r="K25" t="s">
-        <v>187</v>
-      </c>
-      <c r="M25" t="s">
-        <v>186</v>
-      </c>
-      <c r="Q25" t="s">
-        <v>185</v>
-      </c>
-      <c r="V25" t="s">
-        <v>184</v>
-      </c>
       <c r="W25" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="X25" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="26" spans="1:24" x14ac:dyDescent="0.2">
@@ -2715,7 +2715,7 @@
         <v>1</v>
       </c>
       <c r="B26" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="C26">
         <v>2016</v>
@@ -2727,40 +2727,40 @@
         <v>79</v>
       </c>
       <c r="H26" t="s">
+        <v>187</v>
+      </c>
+      <c r="I26" t="s">
         <v>188</v>
       </c>
-      <c r="I26" t="s">
+      <c r="J26" t="s">
+        <v>190</v>
+      </c>
+      <c r="K26" t="s">
+        <v>196</v>
+      </c>
+      <c r="M26" t="s">
+        <v>193</v>
+      </c>
+      <c r="O26" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="P26" t="s">
+        <v>191</v>
+      </c>
+      <c r="S26" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="U26" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="V26" t="s">
         <v>189</v>
       </c>
-      <c r="J26" t="s">
-        <v>191</v>
-      </c>
-      <c r="K26" t="s">
-        <v>197</v>
-      </c>
-      <c r="M26" t="s">
-        <v>194</v>
-      </c>
-      <c r="O26" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="P26" t="s">
-        <v>192</v>
-      </c>
-      <c r="S26" s="1" t="s">
-        <v>196</v>
-      </c>
-      <c r="U26" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="V26" t="s">
-        <v>190</v>
-      </c>
       <c r="W26" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="X26" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="27" spans="1:24" x14ac:dyDescent="0.2">
@@ -2768,7 +2768,7 @@
         <v>1</v>
       </c>
       <c r="B27" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C27">
         <v>2015</v>
@@ -2780,37 +2780,37 @@
         <v>94</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="G27">
         <v>28</v>
       </c>
       <c r="H27" t="s">
+        <v>197</v>
+      </c>
+      <c r="I27" t="s">
         <v>198</v>
       </c>
-      <c r="I27" t="s">
+      <c r="J27" t="s">
         <v>199</v>
       </c>
-      <c r="J27" t="s">
+      <c r="K27" t="s">
+        <v>203</v>
+      </c>
+      <c r="M27" t="s">
+        <v>201</v>
+      </c>
+      <c r="Q27" t="s">
+        <v>202</v>
+      </c>
+      <c r="V27" t="s">
         <v>200</v>
       </c>
-      <c r="K27" t="s">
-        <v>204</v>
-      </c>
-      <c r="M27" t="s">
-        <v>202</v>
-      </c>
-      <c r="Q27" t="s">
-        <v>203</v>
-      </c>
-      <c r="V27" t="s">
-        <v>201</v>
-      </c>
       <c r="W27" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="X27" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
   </sheetData>
@@ -2896,25 +2896,25 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>284</v>
+      </c>
+      <c r="B1" t="s">
+        <v>283</v>
+      </c>
+      <c r="C1" t="s">
+        <v>282</v>
+      </c>
+      <c r="D1" t="s">
+        <v>218</v>
+      </c>
+      <c r="E1" t="s">
+        <v>281</v>
+      </c>
+      <c r="F1" t="s">
+        <v>280</v>
+      </c>
+      <c r="G1" t="s">
         <v>285</v>
-      </c>
-      <c r="B1" t="s">
-        <v>284</v>
-      </c>
-      <c r="C1" t="s">
-        <v>283</v>
-      </c>
-      <c r="D1" t="s">
-        <v>219</v>
-      </c>
-      <c r="E1" t="s">
-        <v>282</v>
-      </c>
-      <c r="F1" t="s">
-        <v>281</v>
-      </c>
-      <c r="G1" t="s">
-        <v>286</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
@@ -2922,19 +2922,19 @@
         <v>2017</v>
       </c>
       <c r="B2" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C2" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D2" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="F2" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="G2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
@@ -2942,19 +2942,19 @@
         <v>2017</v>
       </c>
       <c r="B3" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C3" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="D3" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="F3" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="G3" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
@@ -2965,16 +2965,16 @@
         <v>2017</v>
       </c>
       <c r="C4" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D4" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="F4" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="G4" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
@@ -2982,19 +2982,19 @@
         <v>2018</v>
       </c>
       <c r="B5" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C5" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="D5" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="F5" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="G5" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
@@ -3005,13 +3005,13 @@
         <v>2019</v>
       </c>
       <c r="D6" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="F6" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="G6" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
@@ -3022,13 +3022,13 @@
         <v>2018</v>
       </c>
       <c r="D7" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="F7" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="G7" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
@@ -3039,13 +3039,13 @@
         <v>2017</v>
       </c>
       <c r="D8" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="F8" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="G8" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
@@ -3056,16 +3056,16 @@
         <v>2017</v>
       </c>
       <c r="C9" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="D9" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="F9" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="G9" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
@@ -3076,13 +3076,13 @@
         <v>2017</v>
       </c>
       <c r="D10" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="F10" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="G10" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
@@ -3093,13 +3093,13 @@
         <v>2016</v>
       </c>
       <c r="D11" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="F11" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="G11" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
@@ -3110,13 +3110,13 @@
         <v>2016</v>
       </c>
       <c r="D12" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="F12" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="G12" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
@@ -3127,16 +3127,16 @@
         <v>2017</v>
       </c>
       <c r="C13" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D13" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="F13" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="G13" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
@@ -3147,16 +3147,16 @@
         <v>2013</v>
       </c>
       <c r="C14" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="D14" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="F14" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="G14" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[FEAT] include ajcai video
</commit_message>
<xml_diff>
--- a/data/pubs.xlsx
+++ b/data/pubs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/DoerLBH/Dropbox (Personal)/Git/doerbeta.github.io/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F1307DD-DE88-F546-A13C-A625E308C122}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58643410-55FC-0C47-BD08-E89BCC5A92A0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4240" yWindow="460" windowWidth="28040" windowHeight="19780" xr2:uid="{2388AA68-C25E-CF45-A9DC-089130C49FF2}"/>
+    <workbookView xWindow="38840" yWindow="-6820" windowWidth="33160" windowHeight="19780" xr2:uid="{2388AA68-C25E-CF45-A9DC-089130C49FF2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436" uniqueCount="347">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="439" uniqueCount="350">
   <si>
     <t>title</t>
   </si>
@@ -1075,6 +1075,15 @@
   </si>
   <si>
     <t>https://arxiv.org/abs/2010.11413</t>
+  </si>
+  <si>
+    <t>INTERSPEECH_VoiceID_slides</t>
+  </si>
+  <si>
+    <t>AJCAI_BerlinUCB_slides.pdf</t>
+  </si>
+  <si>
+    <t>https://youtu.be/PsVHObTXtCw</t>
   </si>
 </sst>
 </file>
@@ -1439,8 +1448,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07DC3B69-47EC-374A-9EA9-8E92A8B21FEE}">
   <dimension ref="A1:X28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="U2" sqref="U2"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="T4" sqref="T4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1555,6 +1564,9 @@
       <c r="M2" t="s">
         <v>340</v>
       </c>
+      <c r="R2" t="s">
+        <v>348</v>
+      </c>
       <c r="S2" s="1" t="s">
         <v>341</v>
       </c>
@@ -1611,6 +1623,9 @@
       <c r="S3" s="1" t="s">
         <v>324</v>
       </c>
+      <c r="T3" s="1" t="s">
+        <v>349</v>
+      </c>
       <c r="V3" t="s">
         <v>325</v>
       </c>
@@ -1805,9 +1820,6 @@
       <c r="S7" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="T7" s="1" t="s">
-        <v>64</v>
-      </c>
       <c r="V7" t="s">
         <v>42</v>
       </c>
@@ -1893,6 +1905,9 @@
       <c r="M9" t="s">
         <v>24</v>
       </c>
+      <c r="R9" t="s">
+        <v>347</v>
+      </c>
       <c r="S9" s="1" t="s">
         <v>18</v>
       </c>
@@ -2124,6 +2139,9 @@
       <c r="S13" s="1" t="s">
         <v>52</v>
       </c>
+      <c r="T13" s="1" t="s">
+        <v>64</v>
+      </c>
       <c r="V13" t="s">
         <v>82</v>
       </c>
@@ -2578,7 +2596,7 @@
         <v>214</v>
       </c>
       <c r="G22">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H22" t="s">
         <v>147</v>
@@ -2934,7 +2952,7 @@
     <hyperlink ref="S11" r:id="rId13" xr:uid="{C0259699-F280-044F-8C2F-75CDC809FD84}"/>
     <hyperlink ref="T10" r:id="rId14" xr:uid="{70FB47DE-DBE4-0546-9BCD-A7DF52AECB00}"/>
     <hyperlink ref="T12" r:id="rId15" xr:uid="{A79A47B4-DE43-6349-A3EA-2892C1288230}"/>
-    <hyperlink ref="T7" r:id="rId16" xr:uid="{456B4AB9-81F0-FC4B-A2DF-C5AF2A00DE6D}"/>
+    <hyperlink ref="T13" r:id="rId16" xr:uid="{456B4AB9-81F0-FC4B-A2DF-C5AF2A00DE6D}"/>
     <hyperlink ref="L12" r:id="rId17" xr:uid="{833897A9-E560-8142-BC47-F17858FA9587}"/>
     <hyperlink ref="S12" r:id="rId18" xr:uid="{6BABC62F-6452-374A-9514-5D967BEA7EC4}"/>
     <hyperlink ref="L13" r:id="rId19" xr:uid="{7CC14624-EB38-7844-9223-227BC8C2F65C}"/>
@@ -2984,6 +3002,7 @@
     <hyperlink ref="F21" r:id="rId63" xr:uid="{647A83C8-D1FC-174E-A88A-52525E7B10F7}"/>
     <hyperlink ref="S2" r:id="rId64" xr:uid="{2EAF72F5-CB50-7C4D-B22F-D10C78EB1E84}"/>
     <hyperlink ref="L2" r:id="rId65" xr:uid="{68D24DEE-F463-A54A-A830-2152EA96DED5}"/>
+    <hyperlink ref="T3" r:id="rId66" xr:uid="{B144EDDF-77AE-1B48-BC33-C854247B05C8}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
[DBG] fix slides reference
</commit_message>
<xml_diff>
--- a/data/pubs.xlsx
+++ b/data/pubs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/DoerLBH/Dropbox (Personal)/Git/doerbeta.github.io/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58643410-55FC-0C47-BD08-E89BCC5A92A0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D72F4873-82D7-3648-BC1B-D2D4B0C98C03}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38840" yWindow="-6820" windowWidth="33160" windowHeight="19780" xr2:uid="{2388AA68-C25E-CF45-A9DC-089130C49FF2}"/>
   </bookViews>
@@ -1449,7 +1449,7 @@
   <dimension ref="A1:X28"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="T4" sqref="T4"/>
+      <selection activeCell="R3" sqref="R3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1564,9 +1564,6 @@
       <c r="M2" t="s">
         <v>340</v>
       </c>
-      <c r="R2" t="s">
-        <v>348</v>
-      </c>
       <c r="S2" s="1" t="s">
         <v>341</v>
       </c>
@@ -1619,6 +1616,9 @@
       </c>
       <c r="M3" t="s">
         <v>323</v>
+      </c>
+      <c r="R3" t="s">
+        <v>348</v>
       </c>
       <c r="S3" s="1" t="s">
         <v>324</v>

</xml_diff>

<commit_message>
[FEAT] add V2R youtube
</commit_message>
<xml_diff>
--- a/data/pubs.xlsx
+++ b/data/pubs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/DoerLBH/Dropbox (Personal)/Git/doerbeta.github.io/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81B91370-900F-EF42-82B0-0DC9FEEEB362}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B96D7E43-4051-5245-AF79-7A4BF7D5F9CA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1800" yWindow="460" windowWidth="33160" windowHeight="19780" xr2:uid="{2388AA68-C25E-CF45-A9DC-089130C49FF2}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="439" uniqueCount="350">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="442" uniqueCount="353">
   <si>
     <t>title</t>
   </si>
@@ -1084,6 +1084,15 @@
   </si>
   <si>
     <t>https://youtu.be/PsVHObTXtCw</t>
+  </si>
+  <si>
+    <t>IJCAI_V2R_poster.pdf</t>
+  </si>
+  <si>
+    <t>IJCAI_V2R_slides.pdf</t>
+  </si>
+  <si>
+    <t>https://youtu.be/mEiaFmEq_yQ</t>
   </si>
 </sst>
 </file>
@@ -1449,7 +1458,7 @@
   <dimension ref="A1:X28"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="T12" sqref="T12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2026,10 +2035,18 @@
       <c r="M11" t="s">
         <v>58</v>
       </c>
+      <c r="P11" t="s">
+        <v>350</v>
+      </c>
+      <c r="R11" t="s">
+        <v>351</v>
+      </c>
       <c r="S11" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="T11" s="1"/>
+      <c r="T11" s="1" t="s">
+        <v>352</v>
+      </c>
       <c r="V11" t="s">
         <v>61</v>
       </c>
@@ -2419,7 +2436,7 @@
         <v>215</v>
       </c>
       <c r="G19">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H19" t="s">
         <v>120</v>
@@ -2752,7 +2769,7 @@
         <v>212</v>
       </c>
       <c r="G25">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H25" t="s">
         <v>172</v>
@@ -3003,6 +3020,7 @@
     <hyperlink ref="S2" r:id="rId64" xr:uid="{2EAF72F5-CB50-7C4D-B22F-D10C78EB1E84}"/>
     <hyperlink ref="L2" r:id="rId65" xr:uid="{68D24DEE-F463-A54A-A830-2152EA96DED5}"/>
     <hyperlink ref="T3" r:id="rId66" xr:uid="{B144EDDF-77AE-1B48-BC33-C854247B05C8}"/>
+    <hyperlink ref="T11" r:id="rId67" xr:uid="{AAAE0B81-2DD3-2447-9726-4557F3EC8C6D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
[FEAT] make thumbnails default
</commit_message>
<xml_diff>
--- a/data/pubs.xlsx
+++ b/data/pubs.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11213"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/DoerLBH/Dropbox (Personal)/Git/doerbeta.github.io/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{099B5735-EE11-4644-A219-4C6FAA1DDD83}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7FA342B-5853-A642-9E51-E85D6B430C6D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2260" yWindow="460" windowWidth="33160" windowHeight="19780" xr2:uid="{2388AA68-C25E-CF45-A9DC-089130C49FF2}"/>
   </bookViews>
@@ -1458,7 +1458,7 @@
   <dimension ref="A1:X28"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="I31" sqref="I31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2495,7 +2495,7 @@
         <v>206</v>
       </c>
       <c r="G20">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="H20" t="s">
         <v>130</v>
@@ -2719,7 +2719,7 @@
         <v>210</v>
       </c>
       <c r="G24">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="H24" t="s">
         <v>164</v>
@@ -2769,7 +2769,7 @@
         <v>212</v>
       </c>
       <c r="G25">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H25" t="s">
         <v>172</v>

</xml_diff>

<commit_message>
[FEAT] add field to lab
</commit_message>
<xml_diff>
--- a/data/pubs.xlsx
+++ b/data/pubs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/doerlbh/Dropbox/Git/doerbeta.github.io/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1739991-5514-8B47-B750-E41E8064A48E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53D023C5-D0A2-AA40-BCE0-AD187CF20AE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20260" yWindow="2960" windowWidth="17740" windowHeight="16180" activeTab="1" xr2:uid="{2388AA68-C25E-CF45-A9DC-089130C49FF2}"/>
   </bookViews>
@@ -1134,7 +1134,7 @@
     <t>google</t>
   </si>
   <si>
-    <t>NS-ML-TM-CV</t>
+    <t>NS-ML-TM-CV-SP</t>
   </si>
 </sst>
 </file>
@@ -3125,8 +3125,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00934522-8918-5F4D-855B-4574586BDBC0}">
   <dimension ref="A1:G15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
[DBG] update description and pubs
</commit_message>
<xml_diff>
--- a/data/pubs.xlsx
+++ b/data/pubs.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/DoerLBH/Dropbox (Personal)/Git/doerbeta.github.io/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/doerlbh/Dropbox/Git/doerbeta.github.io/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D87A1C2-1E73-AF43-9EEB-D8AA6D93BE7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99326B7D-0C63-7B4A-BD36-BA5388C04CD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17260" yWindow="740" windowWidth="16880" windowHeight="16040" xr2:uid="{2388AA68-C25E-CF45-A9DC-089130C49FF2}"/>
+    <workbookView xWindow="19320" yWindow="500" windowWidth="16880" windowHeight="16040" xr2:uid="{2388AA68-C25E-CF45-A9DC-089130C49FF2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1502,8 +1502,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07DC3B69-47EC-374A-9EA9-8E92A8B21FEE}">
   <dimension ref="A1:X29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B7" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G32" sqref="G32"/>
+    <sheetView tabSelected="1" topLeftCell="D3" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2714,7 +2714,7 @@
         <v>213</v>
       </c>
       <c r="G23">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="H23" t="s">
         <v>146</v>
@@ -2820,7 +2820,7 @@
         <v>209</v>
       </c>
       <c r="G25">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="H25" t="s">
         <v>163</v>
@@ -2920,7 +2920,7 @@
         <v>212</v>
       </c>
       <c r="G27">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="H27" t="s">
         <v>178</v>
@@ -3023,7 +3023,7 @@
         <v>210</v>
       </c>
       <c r="G29">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="H29" t="s">
         <v>195</v>

</xml_diff>